<commit_message>
Exception of sorcerers spells
</commit_message>
<xml_diff>
--- a/Donjons_et_dragons.xlsx
+++ b/Donjons_et_dragons.xlsx
@@ -5946,20 +5946,20 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="34" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="33" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="34" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="34" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="34" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -17853,10 +17853,10 @@
   <dimension ref="A1:DH35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="AY20" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B23" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="W1" sqref="W1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="BI3" sqref="BI3:BI22"/>
+      <selection pane="bottomRight" activeCell="DH3" sqref="DH3:DH22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -17866,140 +17866,140 @@
   <sheetData>
     <row r="1" spans="1:112">
       <c r="A1" s="194"/>
-      <c r="B1" s="209" t="s">
+      <c r="B1" s="210" t="s">
         <v>385</v>
       </c>
-      <c r="C1" s="209"/>
-      <c r="D1" s="209"/>
-      <c r="E1" s="209"/>
-      <c r="F1" s="210"/>
-      <c r="G1" s="208" t="s">
+      <c r="C1" s="210"/>
+      <c r="D1" s="210"/>
+      <c r="E1" s="210"/>
+      <c r="F1" s="212"/>
+      <c r="G1" s="211" t="s">
         <v>386</v>
       </c>
-      <c r="H1" s="209"/>
-      <c r="I1" s="209"/>
-      <c r="J1" s="209"/>
-      <c r="K1" s="209"/>
-      <c r="L1" s="209"/>
-      <c r="M1" s="209"/>
-      <c r="N1" s="209"/>
-      <c r="O1" s="209"/>
-      <c r="P1" s="209"/>
-      <c r="Q1" s="209"/>
-      <c r="R1" s="209"/>
-      <c r="S1" s="209"/>
+      <c r="H1" s="210"/>
+      <c r="I1" s="210"/>
+      <c r="J1" s="210"/>
+      <c r="K1" s="210"/>
+      <c r="L1" s="210"/>
+      <c r="M1" s="210"/>
+      <c r="N1" s="210"/>
+      <c r="O1" s="210"/>
+      <c r="P1" s="210"/>
+      <c r="Q1" s="210"/>
+      <c r="R1" s="210"/>
+      <c r="S1" s="210"/>
       <c r="T1" s="182"/>
-      <c r="U1" s="209" t="s">
+      <c r="U1" s="210" t="s">
         <v>387</v>
       </c>
-      <c r="V1" s="209"/>
-      <c r="W1" s="209"/>
-      <c r="X1" s="209"/>
-      <c r="Y1" s="209"/>
-      <c r="Z1" s="209"/>
-      <c r="AA1" s="209"/>
-      <c r="AB1" s="209"/>
-      <c r="AC1" s="209"/>
-      <c r="AD1" s="209"/>
-      <c r="AE1" s="209"/>
-      <c r="AF1" s="209"/>
+      <c r="V1" s="210"/>
+      <c r="W1" s="210"/>
+      <c r="X1" s="210"/>
+      <c r="Y1" s="210"/>
+      <c r="Z1" s="210"/>
+      <c r="AA1" s="210"/>
+      <c r="AB1" s="210"/>
+      <c r="AC1" s="210"/>
+      <c r="AD1" s="210"/>
+      <c r="AE1" s="210"/>
+      <c r="AF1" s="210"/>
       <c r="AG1" s="165"/>
-      <c r="AH1" s="208" t="s">
+      <c r="AH1" s="211" t="s">
         <v>388</v>
       </c>
-      <c r="AI1" s="209"/>
-      <c r="AJ1" s="209"/>
-      <c r="AK1" s="209"/>
-      <c r="AL1" s="209"/>
-      <c r="AM1" s="209"/>
-      <c r="AN1" s="209"/>
-      <c r="AO1" s="209"/>
-      <c r="AP1" s="209"/>
-      <c r="AQ1" s="209"/>
-      <c r="AR1" s="209"/>
-      <c r="AS1" s="210"/>
+      <c r="AI1" s="210"/>
+      <c r="AJ1" s="210"/>
+      <c r="AK1" s="210"/>
+      <c r="AL1" s="210"/>
+      <c r="AM1" s="210"/>
+      <c r="AN1" s="210"/>
+      <c r="AO1" s="210"/>
+      <c r="AP1" s="210"/>
+      <c r="AQ1" s="210"/>
+      <c r="AR1" s="210"/>
+      <c r="AS1" s="212"/>
       <c r="AT1" s="165"/>
-      <c r="AU1" s="211" t="s">
+      <c r="AU1" s="209" t="s">
         <v>389</v>
       </c>
-      <c r="AV1" s="211"/>
-      <c r="AW1" s="211"/>
-      <c r="AX1" s="211"/>
-      <c r="AY1" s="211"/>
-      <c r="AZ1" s="211"/>
-      <c r="BA1" s="211"/>
-      <c r="BB1" s="211"/>
-      <c r="BC1" s="211"/>
-      <c r="BD1" s="211"/>
-      <c r="BE1" s="211"/>
-      <c r="BF1" s="211"/>
-      <c r="BG1" s="211"/>
-      <c r="BH1" s="211"/>
+      <c r="AV1" s="209"/>
+      <c r="AW1" s="209"/>
+      <c r="AX1" s="209"/>
+      <c r="AY1" s="209"/>
+      <c r="AZ1" s="209"/>
+      <c r="BA1" s="209"/>
+      <c r="BB1" s="209"/>
+      <c r="BC1" s="209"/>
+      <c r="BD1" s="209"/>
+      <c r="BE1" s="209"/>
+      <c r="BF1" s="209"/>
+      <c r="BG1" s="209"/>
+      <c r="BH1" s="209"/>
       <c r="BI1" s="178"/>
-      <c r="BJ1" s="208" t="s">
+      <c r="BJ1" s="211" t="s">
         <v>390</v>
       </c>
-      <c r="BK1" s="209"/>
+      <c r="BK1" s="210"/>
       <c r="BL1" s="182"/>
-      <c r="BM1" s="209" t="s">
+      <c r="BM1" s="210" t="s">
         <v>391</v>
       </c>
-      <c r="BN1" s="209"/>
-      <c r="BO1" s="209"/>
-      <c r="BP1" s="209"/>
-      <c r="BQ1" s="209"/>
-      <c r="BR1" s="209"/>
-      <c r="BS1" s="209"/>
-      <c r="BT1" s="209"/>
-      <c r="BU1" s="209"/>
-      <c r="BV1" s="209"/>
-      <c r="BW1" s="209"/>
-      <c r="BX1" s="209"/>
+      <c r="BN1" s="210"/>
+      <c r="BO1" s="210"/>
+      <c r="BP1" s="210"/>
+      <c r="BQ1" s="210"/>
+      <c r="BR1" s="210"/>
+      <c r="BS1" s="210"/>
+      <c r="BT1" s="210"/>
+      <c r="BU1" s="210"/>
+      <c r="BV1" s="210"/>
+      <c r="BW1" s="210"/>
+      <c r="BX1" s="210"/>
       <c r="BY1" s="165"/>
-      <c r="BZ1" s="208" t="s">
+      <c r="BZ1" s="211" t="s">
         <v>393</v>
       </c>
-      <c r="CA1" s="209"/>
-      <c r="CB1" s="209"/>
-      <c r="CC1" s="209"/>
-      <c r="CD1" s="209"/>
+      <c r="CA1" s="210"/>
+      <c r="CB1" s="210"/>
+      <c r="CC1" s="210"/>
+      <c r="CD1" s="210"/>
       <c r="CE1" s="182"/>
-      <c r="CF1" s="208" t="s">
+      <c r="CF1" s="211" t="s">
         <v>12</v>
       </c>
-      <c r="CG1" s="209"/>
-      <c r="CH1" s="209"/>
-      <c r="CI1" s="209"/>
-      <c r="CJ1" s="209"/>
-      <c r="CK1" s="209"/>
-      <c r="CL1" s="209"/>
+      <c r="CG1" s="210"/>
+      <c r="CH1" s="210"/>
+      <c r="CI1" s="210"/>
+      <c r="CJ1" s="210"/>
+      <c r="CK1" s="210"/>
+      <c r="CL1" s="210"/>
       <c r="CM1" s="182"/>
-      <c r="CN1" s="209" t="s">
+      <c r="CN1" s="210" t="s">
         <v>394</v>
       </c>
-      <c r="CO1" s="209"/>
-      <c r="CP1" s="209"/>
-      <c r="CQ1" s="209"/>
-      <c r="CR1" s="209"/>
-      <c r="CS1" s="209"/>
-      <c r="CT1" s="209"/>
-      <c r="CU1" s="209"/>
+      <c r="CO1" s="210"/>
+      <c r="CP1" s="210"/>
+      <c r="CQ1" s="210"/>
+      <c r="CR1" s="210"/>
+      <c r="CS1" s="210"/>
+      <c r="CT1" s="210"/>
+      <c r="CU1" s="210"/>
       <c r="CV1" s="165"/>
-      <c r="CW1" s="212" t="s">
+      <c r="CW1" s="208" t="s">
         <v>395</v>
       </c>
-      <c r="CX1" s="211"/>
-      <c r="CY1" s="211"/>
+      <c r="CX1" s="209"/>
+      <c r="CY1" s="209"/>
       <c r="CZ1" s="192"/>
-      <c r="DA1" s="209" t="s">
+      <c r="DA1" s="210" t="s">
         <v>392</v>
       </c>
-      <c r="DB1" s="209"/>
-      <c r="DC1" s="209"/>
-      <c r="DD1" s="209"/>
-      <c r="DE1" s="209"/>
-      <c r="DF1" s="209"/>
-      <c r="DG1" s="209"/>
+      <c r="DB1" s="210"/>
+      <c r="DC1" s="210"/>
+      <c r="DD1" s="210"/>
+      <c r="DE1" s="210"/>
+      <c r="DF1" s="210"/>
+      <c r="DG1" s="210"/>
       <c r="DH1" s="203"/>
     </row>
     <row r="2" spans="1:112" s="129" customFormat="1" ht="39" customHeight="1">
@@ -18864,16 +18864,14 @@
 ""Capacities"":"""&amp;DB3&amp;""",
 ""MinorSpells"": "&amp;DC3&amp;",
 ""Spells"": "&amp;DD3&amp;",
-""Locations"": "&amp;DE3&amp;",
-""LocationLevel"": "&amp;DF3&amp;",
+""Locations"": {"""&amp;DF3&amp;""":"&amp;DE3&amp;"},
 ""Invocations"": "&amp;DG3&amp;"
 },"</f>
         <v>"WIZARD-1" : {
 "Capacities":"Patron d'Outremonde, Magie de pacte",
 "MinorSpells": 2,
 "Spells": 2,
-"Locations": 1,
-"LocationLevel": 1,
+"Locations": {"1":1},
 "Invocations": 0
 },</v>
       </c>
@@ -19366,21 +19364,19 @@
 ""Capacities"":"""&amp;DB4&amp;""",
 ""MinorSpells"": "&amp;DC4&amp;",
 ""Spells"": "&amp;DD4&amp;",
-""Locations"": "&amp;DE4&amp;",
-""LocationLevel"": "&amp;DF4&amp;",
+""Locations"": {"""&amp;DF4&amp;""":"&amp;DE4&amp;"},
 ""Invocations"": "&amp;DG4&amp;"
 },"</f>
         <v>"WIZARD-2" : {
 "Capacities":"Invocations occultes",
 "MinorSpells": 2,
 "Spells": 3,
-"Locations": 2,
-"LocationLevel": 1,
+"Locations": {"1":2},
 "Invocations": 2
 },</v>
       </c>
     </row>
-    <row r="5" spans="1:112" ht="293.25">
+    <row r="5" spans="1:112" ht="280.5">
       <c r="A5" s="179">
         <v>3</v>
       </c>
@@ -19830,8 +19826,7 @@
 "Capacities":"Faveur de pacte",
 "MinorSpells": 2,
 "Spells": 4,
-"Locations": 2,
-"LocationLevel": 2,
+"Locations": {"2":2},
 "Invocations": 2
 },</v>
       </c>
@@ -20286,13 +20281,12 @@
 "Capacities":"Amélioration de caractéristiques",
 "MinorSpells": 3,
 "Spells": 5,
-"Locations": 2,
-"LocationLevel": 2,
+"Locations": {"2":2},
 "Invocations": 2
 },</v>
       </c>
     </row>
-    <row r="7" spans="1:112" ht="293.25">
+    <row r="7" spans="1:112" ht="280.5">
       <c r="A7" s="179">
         <v>5</v>
       </c>
@@ -20742,8 +20736,7 @@
 "Capacities":"-",
 "MinorSpells": 3,
 "Spells": 6,
-"Locations": 2,
-"LocationLevel": 3,
+"Locations": {"3":2},
 "Invocations": 3
 },</v>
       </c>
@@ -21198,13 +21191,12 @@
 "Capacities":"Capacité de patron d'Outremonde",
 "MinorSpells": 3,
 "Spells": 7,
-"Locations": 2,
-"LocationLevel": 3,
+"Locations": {"3":2},
 "Invocations": 3
 },</v>
       </c>
     </row>
-    <row r="9" spans="1:112" ht="293.25">
+    <row r="9" spans="1:112" ht="267.75">
       <c r="A9" s="179">
         <v>7</v>
       </c>
@@ -21599,7 +21591,16 @@
         <v>0</v>
       </c>
       <c r="CV9" s="5" t="str">
-        <f t="shared" si="4"/>
+        <f>""""&amp;$CN$1&amp;"-"&amp;$A9&amp;""" : {
+""Capacities"":"""&amp;CO9&amp;""",
+""Spells"":"&amp;CP9&amp;",
+""Locations"": {
+""1"":"&amp;CQ9&amp;",
+""2"":"&amp;CR9&amp;",
+""3"":"&amp;CS9&amp;",
+""4"":"&amp;CT9&amp;",
+""5"":"&amp;CU9&amp;"}
+},"</f>
         <v>"PROWLER-7" : {
 "Capacities":"Capacité de l'archétype de rôdeur",
 "Spells":5,
@@ -21654,8 +21655,7 @@
 "Capacities":"-",
 "MinorSpells": 3,
 "Spells": 8,
-"Locations": 2,
-"LocationLevel": 4,
+"Locations": {"4":2},
 "Invocations": 4
 },</v>
       </c>
@@ -22110,13 +22110,12 @@
 "Capacities":"Amélioration de caractéristiques",
 "MinorSpells": 3,
 "Spells": 9,
-"Locations": 2,
-"LocationLevel": 4,
+"Locations": {"4":2},
 "Invocations": 4
 },</v>
       </c>
     </row>
-    <row r="11" spans="1:112" ht="293.25">
+    <row r="11" spans="1:112" ht="267.75">
       <c r="A11" s="179">
         <v>9</v>
       </c>
@@ -22568,8 +22567,7 @@
 "Capacities":"-",
 "MinorSpells": 3,
 "Spells": 10,
-"Locations": 2,
-"LocationLevel": 5,
+"Locations": {"5":2},
 "Invocations": 5
 },</v>
       </c>
@@ -23024,13 +23022,12 @@
 "Capacities":"Capacité de patron d'Outremonde",
 "MinorSpells": 4,
 "Spells": 10,
-"Locations": 2,
-"LocationLevel": 5,
+"Locations": {"5":2},
 "Invocations": 5
 },</v>
       </c>
     </row>
-    <row r="13" spans="1:112" ht="293.25">
+    <row r="13" spans="1:112" ht="267.75">
       <c r="A13" s="179">
         <v>11</v>
       </c>
@@ -23482,13 +23479,12 @@
 "Capacities":"Arcanum mystique (niveau 6)",
 "MinorSpells": 4,
 "Spells": 11,
-"Locations": 3,
-"LocationLevel": 5,
+"Locations": {"5":3},
 "Invocations": 5
 },</v>
       </c>
     </row>
-    <row r="14" spans="1:112" ht="293.25">
+    <row r="14" spans="1:112" ht="306">
       <c r="A14" s="180">
         <v>12</v>
       </c>
@@ -23938,13 +23934,12 @@
 "Capacities":"Amélioration de caractéristiques",
 "MinorSpells": 4,
 "Spells": 11,
-"Locations": 3,
-"LocationLevel": 5,
+"Locations": {"5":3},
 "Invocations": 6
 },</v>
       </c>
     </row>
-    <row r="15" spans="1:112" ht="293.25">
+    <row r="15" spans="1:112" ht="267.75">
       <c r="A15" s="179">
         <v>13</v>
       </c>
@@ -24394,8 +24389,7 @@
 "Capacities":"Arcanum mystique (niveau 7)",
 "MinorSpells": 4,
 "Spells": 12,
-"Locations": 3,
-"LocationLevel": 5,
+"Locations": {"5":3},
 "Invocations": 6
 },</v>
       </c>
@@ -24850,13 +24844,12 @@
 "Capacities":"Capacité de patron d'Outremonde",
 "MinorSpells": 4,
 "Spells": 12,
-"Locations": 3,
-"LocationLevel": 5,
+"Locations": {"5":3},
 "Invocations": 6
 },</v>
       </c>
     </row>
-    <row r="17" spans="1:112" ht="293.25">
+    <row r="17" spans="1:112" ht="267.75">
       <c r="A17" s="179">
         <v>15</v>
       </c>
@@ -25306,13 +25299,12 @@
 "Capacities":"Arcanum mystique (niveau 8)",
 "MinorSpells": 4,
 "Spells": 13,
-"Locations": 3,
-"LocationLevel": 5,
+"Locations": {"5":3},
 "Invocations": 7
 },</v>
       </c>
     </row>
-    <row r="18" spans="1:112" ht="293.25">
+    <row r="18" spans="1:112" ht="306">
       <c r="A18" s="180">
         <v>16</v>
       </c>
@@ -25762,8 +25754,7 @@
 "Capacities":"Amélioration de caractéristiques",
 "MinorSpells": 4,
 "Spells": 13,
-"Locations": 3,
-"LocationLevel": 5,
+"Locations": {"5":3},
 "Invocations": 7
 },</v>
       </c>
@@ -26218,8 +26209,7 @@
 "Capacities":"Arcanum mystique (niveau 9)",
 "MinorSpells": 4,
 "Spells": 14,
-"Locations": 4,
-"LocationLevel": 5,
+"Locations": {"5":4},
 "Invocations": 7
 },</v>
       </c>
@@ -26674,13 +26664,12 @@
 "Capacities":"-",
 "MinorSpells": 4,
 "Spells": 14,
-"Locations": 4,
-"LocationLevel": 5,
+"Locations": {"5":4},
 "Invocations": 8
 },</v>
       </c>
     </row>
-    <row r="21" spans="1:112" ht="293.25">
+    <row r="21" spans="1:112" ht="306">
       <c r="A21" s="179">
         <v>19</v>
       </c>
@@ -27132,8 +27121,7 @@
 "Capacities":"Amélioration de caractéristiques",
 "MinorSpells": 4,
 "Spells": 15,
-"Locations": 4,
-"LocationLevel": 5,
+"Locations": {"5":4},
 "Invocations": 8
 },</v>
       </c>
@@ -27588,8 +27576,7 @@
 "Capacities":"Maître de l'occulte",
 "MinorSpells": 4,
 "Spells": 15,
-"Locations": 4,
-"LocationLevel": 5,
+"Locations": {"5":4},
 "Invocations": 8
 },</v>
       </c>
@@ -29647,147 +29634,132 @@
 "Capacities":"Patron d'Outremonde, Magie de pacte",
 "MinorSpells": 2,
 "Spells": 2,
-"Locations": 1,
-"LocationLevel": 1,
+"Locations": {"1":1},
 "Invocations": 0
 },"WIZARD-2" : {
 "Capacities":"Invocations occultes",
 "MinorSpells": 2,
 "Spells": 3,
-"Locations": 2,
-"LocationLevel": 1,
+"Locations": {"1":2},
 "Invocations": 2
 },"WIZARD-3" : {
 "Capacities":"Faveur de pacte",
 "MinorSpells": 2,
 "Spells": 4,
-"Locations": 2,
-"LocationLevel": 2,
+"Locations": {"2":2},
 "Invocations": 2
 },"WIZARD-4" : {
 "Capacities":"Amélioration de caractéristiques",
 "MinorSpells": 3,
 "Spells": 5,
-"Locations": 2,
-"LocationLevel": 2,
+"Locations": {"2":2},
 "Invocations": 2
 },"WIZARD-5" : {
 "Capacities":"-",
 "MinorSpells": 3,
 "Spells": 6,
-"Locations": 2,
-"LocationLevel": 3,
+"Locations": {"3":2},
 "Invocations": 3
 },"WIZARD-6" : {
 "Capacities":"Capacité de patron d'Outremonde",
 "MinorSpells": 3,
 "Spells": 7,
-"Locations": 2,
-"LocationLevel": 3,
+"Locations": {"3":2},
 "Invocations": 3
 },"WIZARD-7" : {
 "Capacities":"-",
 "MinorSpells": 3,
 "Spells": 8,
-"Locations": 2,
-"LocationLevel": 4,
+"Locations": {"4":2},
 "Invocations": 4
 },"WIZARD-8" : {
 "Capacities":"Amélioration de caractéristiques",
 "MinorSpells": 3,
 "Spells": 9,
-"Locations": 2,
-"LocationLevel": 4,
+"Locations": {"4":2},
 "Invocations": 4
 },"WIZARD-9" : {
 "Capacities":"-",
 "MinorSpells": 3,
 "Spells": 10,
-"Locations": 2,
-"LocationLevel": 5,
+"Locations": {"5":2},
 "Invocations": 5
 },"WIZARD-10" : {
 "Capacities":"Capacité de patron d'Outremonde",
 "MinorSpells": 4,
 "Spells": 10,
-"Locations": 2,
-"LocationLevel": 5,
+"Locations": {"5":2},
 "Invocations": 5
 },"WIZARD-11" : {
 "Capacities":"Arcanum mystique (niveau 6)",
 "MinorSpells": 4,
 "Spells": 11,
-"Locations": 3,
-"LocationLevel": 5,
+"Locations": {"5":3},
 "Invocations": 5
 },"WIZARD-12" : {
 "Capacities":"Amélioration de caractéristiques",
 "MinorSpells": 4,
 "Spells": 11,
-"Locations": 3,
-"LocationLevel": 5,
+"Locations": {"5":3},
 "Invocations": 6
 },"WIZARD-13" : {
 "Capacities":"Arcanum mystique (niveau 7)",
 "MinorSpells": 4,
 "Spells": 12,
-"Locations": 3,
-"LocationLevel": 5,
+"Locations": {"5":3},
 "Invocations": 6
 },"WIZARD-14" : {
 "Capacities":"Capacité de patron d'Outremonde",
 "MinorSpells": 4,
 "Spells": 12,
-"Locations": 3,
-"LocationLevel": 5,
+"Locations": {"5":3},
 "Invocations": 6
 },"WIZARD-15" : {
 "Capacities":"Arcanum mystique (niveau 8)",
 "MinorSpells": 4,
 "Spells": 13,
-"Locations": 3,
-"LocationLevel": 5,
+"Locations": {"5":3},
 "Invocations": 7
 },"WIZARD-16" : {
 "Capacities":"Amélioration de caractéristiques",
 "MinorSpells": 4,
 "Spells": 13,
-"Locations": 3,
-"LocationLevel": 5,
+"Locations": {"5":3},
 "Invocations": 7
 },"WIZARD-17" : {
 "Capacities":"Arcanum mystique (niveau 9)",
 "MinorSpells": 4,
 "Spells": 14,
-"Locations": 4,
-"LocationLevel": 5,
+"Locations": {"5":4},
 "Invocations": 7
 },"WIZARD-18" : {
 "Capacities":"-",
 "MinorSpells": 4,
 "Spells": 14,
-"Locations": 4,
-"LocationLevel": 5,
+"Locations": {"5":4},
 "Invocations": 8
 },"WIZARD-19" : {
 "Capacities":"Amélioration de caractéristiques",
 "MinorSpells": 4,
 "Spells": 15,
-"Locations": 4,
-"LocationLevel": 5,
+"Locations": {"5":4},
 "Invocations": 8
 },"WIZARD-20" : {
 "Capacities":"Maître de l'occulte",
 "MinorSpells": 4,
 "Spells": 15,
-"Locations": 4,
-"LocationLevel": 5,
+"Locations": {"5":4},
 "Invocations": 8
 },</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="AH1:AS1"/>
+    <mergeCell ref="G1:S1"/>
+    <mergeCell ref="AU1:BH1"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="U1:AF1"/>
     <mergeCell ref="CW1:CY1"/>
     <mergeCell ref="DA1:DG1"/>
     <mergeCell ref="CF1:CL1"/>
@@ -29795,11 +29767,6 @@
     <mergeCell ref="BJ1:BK1"/>
     <mergeCell ref="BM1:BX1"/>
     <mergeCell ref="BZ1:CD1"/>
-    <mergeCell ref="AH1:AS1"/>
-    <mergeCell ref="G1:S1"/>
-    <mergeCell ref="AU1:BH1"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="U1:AF1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Weapons icons + Ammunitions
</commit_message>
<xml_diff>
--- a/Donjons_et_dragons.xlsx
+++ b/Donjons_et_dragons.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7515" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7515" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Niveaux" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,6 @@
     <sheet name="Moine" sheetId="8" r:id="rId19"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -10899,20 +10898,29 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="34" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="34" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="34" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="34" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -10937,15 +10945,6 @@
     </xf>
     <xf numFmtId="0" fontId="32" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -59033,7 +59032,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="L2" sqref="L2:L13"/>
     </sheetView>
   </sheetViews>
@@ -62282,140 +62281,140 @@
   <sheetData>
     <row r="1" spans="1:112">
       <c r="A1" s="194"/>
-      <c r="B1" s="213" t="s">
+      <c r="B1" s="217" t="s">
         <v>385</v>
       </c>
-      <c r="C1" s="213"/>
-      <c r="D1" s="213"/>
-      <c r="E1" s="213"/>
-      <c r="F1" s="214"/>
-      <c r="G1" s="212" t="s">
+      <c r="C1" s="217"/>
+      <c r="D1" s="217"/>
+      <c r="E1" s="217"/>
+      <c r="F1" s="219"/>
+      <c r="G1" s="218" t="s">
         <v>386</v>
       </c>
-      <c r="H1" s="213"/>
-      <c r="I1" s="213"/>
-      <c r="J1" s="213"/>
-      <c r="K1" s="213"/>
-      <c r="L1" s="213"/>
-      <c r="M1" s="213"/>
-      <c r="N1" s="213"/>
-      <c r="O1" s="213"/>
-      <c r="P1" s="213"/>
-      <c r="Q1" s="213"/>
-      <c r="R1" s="213"/>
-      <c r="S1" s="213"/>
+      <c r="H1" s="217"/>
+      <c r="I1" s="217"/>
+      <c r="J1" s="217"/>
+      <c r="K1" s="217"/>
+      <c r="L1" s="217"/>
+      <c r="M1" s="217"/>
+      <c r="N1" s="217"/>
+      <c r="O1" s="217"/>
+      <c r="P1" s="217"/>
+      <c r="Q1" s="217"/>
+      <c r="R1" s="217"/>
+      <c r="S1" s="217"/>
       <c r="T1" s="182"/>
-      <c r="U1" s="213" t="s">
+      <c r="U1" s="217" t="s">
         <v>387</v>
       </c>
-      <c r="V1" s="213"/>
-      <c r="W1" s="213"/>
-      <c r="X1" s="213"/>
-      <c r="Y1" s="213"/>
-      <c r="Z1" s="213"/>
-      <c r="AA1" s="213"/>
-      <c r="AB1" s="213"/>
-      <c r="AC1" s="213"/>
-      <c r="AD1" s="213"/>
-      <c r="AE1" s="213"/>
-      <c r="AF1" s="213"/>
+      <c r="V1" s="217"/>
+      <c r="W1" s="217"/>
+      <c r="X1" s="217"/>
+      <c r="Y1" s="217"/>
+      <c r="Z1" s="217"/>
+      <c r="AA1" s="217"/>
+      <c r="AB1" s="217"/>
+      <c r="AC1" s="217"/>
+      <c r="AD1" s="217"/>
+      <c r="AE1" s="217"/>
+      <c r="AF1" s="217"/>
       <c r="AG1" s="165"/>
-      <c r="AH1" s="212" t="s">
+      <c r="AH1" s="218" t="s">
         <v>388</v>
       </c>
-      <c r="AI1" s="213"/>
-      <c r="AJ1" s="213"/>
-      <c r="AK1" s="213"/>
-      <c r="AL1" s="213"/>
-      <c r="AM1" s="213"/>
-      <c r="AN1" s="213"/>
-      <c r="AO1" s="213"/>
-      <c r="AP1" s="213"/>
-      <c r="AQ1" s="213"/>
-      <c r="AR1" s="213"/>
-      <c r="AS1" s="214"/>
+      <c r="AI1" s="217"/>
+      <c r="AJ1" s="217"/>
+      <c r="AK1" s="217"/>
+      <c r="AL1" s="217"/>
+      <c r="AM1" s="217"/>
+      <c r="AN1" s="217"/>
+      <c r="AO1" s="217"/>
+      <c r="AP1" s="217"/>
+      <c r="AQ1" s="217"/>
+      <c r="AR1" s="217"/>
+      <c r="AS1" s="219"/>
       <c r="AT1" s="165"/>
-      <c r="AU1" s="215" t="s">
+      <c r="AU1" s="216" t="s">
         <v>389</v>
       </c>
-      <c r="AV1" s="215"/>
-      <c r="AW1" s="215"/>
-      <c r="AX1" s="215"/>
-      <c r="AY1" s="215"/>
-      <c r="AZ1" s="215"/>
-      <c r="BA1" s="215"/>
-      <c r="BB1" s="215"/>
-      <c r="BC1" s="215"/>
-      <c r="BD1" s="215"/>
-      <c r="BE1" s="215"/>
-      <c r="BF1" s="215"/>
-      <c r="BG1" s="215"/>
-      <c r="BH1" s="215"/>
+      <c r="AV1" s="216"/>
+      <c r="AW1" s="216"/>
+      <c r="AX1" s="216"/>
+      <c r="AY1" s="216"/>
+      <c r="AZ1" s="216"/>
+      <c r="BA1" s="216"/>
+      <c r="BB1" s="216"/>
+      <c r="BC1" s="216"/>
+      <c r="BD1" s="216"/>
+      <c r="BE1" s="216"/>
+      <c r="BF1" s="216"/>
+      <c r="BG1" s="216"/>
+      <c r="BH1" s="216"/>
       <c r="BI1" s="178"/>
-      <c r="BJ1" s="212" t="s">
+      <c r="BJ1" s="218" t="s">
         <v>390</v>
       </c>
-      <c r="BK1" s="213"/>
+      <c r="BK1" s="217"/>
       <c r="BL1" s="182"/>
-      <c r="BM1" s="213" t="s">
+      <c r="BM1" s="217" t="s">
         <v>391</v>
       </c>
-      <c r="BN1" s="213"/>
-      <c r="BO1" s="213"/>
-      <c r="BP1" s="213"/>
-      <c r="BQ1" s="213"/>
-      <c r="BR1" s="213"/>
-      <c r="BS1" s="213"/>
-      <c r="BT1" s="213"/>
-      <c r="BU1" s="213"/>
-      <c r="BV1" s="213"/>
-      <c r="BW1" s="213"/>
-      <c r="BX1" s="213"/>
+      <c r="BN1" s="217"/>
+      <c r="BO1" s="217"/>
+      <c r="BP1" s="217"/>
+      <c r="BQ1" s="217"/>
+      <c r="BR1" s="217"/>
+      <c r="BS1" s="217"/>
+      <c r="BT1" s="217"/>
+      <c r="BU1" s="217"/>
+      <c r="BV1" s="217"/>
+      <c r="BW1" s="217"/>
+      <c r="BX1" s="217"/>
       <c r="BY1" s="165"/>
-      <c r="BZ1" s="212" t="s">
+      <c r="BZ1" s="218" t="s">
         <v>393</v>
       </c>
-      <c r="CA1" s="213"/>
-      <c r="CB1" s="213"/>
-      <c r="CC1" s="213"/>
-      <c r="CD1" s="213"/>
+      <c r="CA1" s="217"/>
+      <c r="CB1" s="217"/>
+      <c r="CC1" s="217"/>
+      <c r="CD1" s="217"/>
       <c r="CE1" s="182"/>
-      <c r="CF1" s="212" t="s">
+      <c r="CF1" s="218" t="s">
         <v>12</v>
       </c>
-      <c r="CG1" s="213"/>
-      <c r="CH1" s="213"/>
-      <c r="CI1" s="213"/>
-      <c r="CJ1" s="213"/>
-      <c r="CK1" s="213"/>
-      <c r="CL1" s="213"/>
+      <c r="CG1" s="217"/>
+      <c r="CH1" s="217"/>
+      <c r="CI1" s="217"/>
+      <c r="CJ1" s="217"/>
+      <c r="CK1" s="217"/>
+      <c r="CL1" s="217"/>
       <c r="CM1" s="182"/>
-      <c r="CN1" s="213" t="s">
+      <c r="CN1" s="217" t="s">
         <v>394</v>
       </c>
-      <c r="CO1" s="213"/>
-      <c r="CP1" s="213"/>
-      <c r="CQ1" s="213"/>
-      <c r="CR1" s="213"/>
-      <c r="CS1" s="213"/>
-      <c r="CT1" s="213"/>
-      <c r="CU1" s="213"/>
+      <c r="CO1" s="217"/>
+      <c r="CP1" s="217"/>
+      <c r="CQ1" s="217"/>
+      <c r="CR1" s="217"/>
+      <c r="CS1" s="217"/>
+      <c r="CT1" s="217"/>
+      <c r="CU1" s="217"/>
       <c r="CV1" s="165"/>
-      <c r="CW1" s="216" t="s">
+      <c r="CW1" s="215" t="s">
         <v>395</v>
       </c>
-      <c r="CX1" s="215"/>
-      <c r="CY1" s="215"/>
+      <c r="CX1" s="216"/>
+      <c r="CY1" s="216"/>
       <c r="CZ1" s="192"/>
-      <c r="DA1" s="213" t="s">
+      <c r="DA1" s="217" t="s">
         <v>392</v>
       </c>
-      <c r="DB1" s="213"/>
-      <c r="DC1" s="213"/>
-      <c r="DD1" s="213"/>
-      <c r="DE1" s="213"/>
-      <c r="DF1" s="213"/>
-      <c r="DG1" s="213"/>
+      <c r="DB1" s="217"/>
+      <c r="DC1" s="217"/>
+      <c r="DD1" s="217"/>
+      <c r="DE1" s="217"/>
+      <c r="DF1" s="217"/>
+      <c r="DG1" s="217"/>
       <c r="DH1" s="203"/>
     </row>
     <row r="2" spans="1:112" s="129" customFormat="1" ht="15" customHeight="1">
@@ -76955,6 +76954,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="AH1:AS1"/>
+    <mergeCell ref="G1:S1"/>
+    <mergeCell ref="AU1:BH1"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="U1:AF1"/>
     <mergeCell ref="CW1:CY1"/>
     <mergeCell ref="DA1:DG1"/>
     <mergeCell ref="CF1:CL1"/>
@@ -76962,11 +76966,6 @@
     <mergeCell ref="BJ1:BK1"/>
     <mergeCell ref="BM1:BX1"/>
     <mergeCell ref="BZ1:CD1"/>
-    <mergeCell ref="AH1:AS1"/>
-    <mergeCell ref="G1:S1"/>
-    <mergeCell ref="AU1:BH1"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="U1:AF1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -77450,8 +77449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C28" workbookViewId="0">
-      <selection activeCell="J38" sqref="J38:J42"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -77499,16 +77498,16 @@
       <c r="L1" s="115"/>
     </row>
     <row r="2" spans="1:13" ht="15" customHeight="1">
-      <c r="A2" s="217" t="s">
+      <c r="A2" s="220" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="218"/>
-      <c r="C2" s="218"/>
-      <c r="D2" s="218"/>
-      <c r="E2" s="218"/>
-      <c r="F2" s="218"/>
-      <c r="G2" s="218"/>
-      <c r="H2" s="219"/>
+      <c r="B2" s="221"/>
+      <c r="C2" s="221"/>
+      <c r="D2" s="221"/>
+      <c r="E2" s="221"/>
+      <c r="F2" s="221"/>
+      <c r="G2" s="221"/>
+      <c r="H2" s="222"/>
       <c r="I2" s="116"/>
       <c r="J2" s="116"/>
       <c r="K2" s="117"/>
@@ -77586,11 +77585,11 @@
       <c r="C4" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="226" t="str">
+      <c r="D4" s="213" t="str">
         <f t="shared" ref="D4:D12" si="2">LEFT(C4,FIND(" ",C4))</f>
         <v xml:space="preserve">1d4 </v>
       </c>
-      <c r="E4" s="226" t="str">
+      <c r="E4" s="213" t="str">
         <f t="shared" ref="E4:E12" si="3">PROPER(RIGHT(C4,LEN(C4)-LEN(D4)))</f>
         <v>Perforant</v>
       </c>
@@ -77701,11 +77700,11 @@
       <c r="C6" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="D6" s="226" t="str">
+      <c r="D6" s="213" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">1d6 </v>
       </c>
-      <c r="E6" s="226" t="str">
+      <c r="E6" s="213" t="str">
         <f t="shared" si="3"/>
         <v>Tranchant</v>
       </c>
@@ -77807,11 +77806,11 @@
       <c r="C8" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="226" t="str">
+      <c r="D8" s="213" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">1d6 </v>
       </c>
-      <c r="E8" s="226" t="str">
+      <c r="E8" s="213" t="str">
         <f t="shared" si="3"/>
         <v>Perforant</v>
       </c>
@@ -77913,11 +77912,11 @@
       <c r="C10" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="226" t="str">
+      <c r="D10" s="213" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">1d6 </v>
       </c>
-      <c r="E10" s="226" t="str">
+      <c r="E10" s="213" t="str">
         <f t="shared" si="3"/>
         <v>Contondant</v>
       </c>
@@ -78019,15 +78018,15 @@
       <c r="C12" s="36" t="s">
         <v>56</v>
       </c>
-      <c r="D12" s="226" t="str">
+      <c r="D12" s="213" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">1d4 </v>
       </c>
-      <c r="E12" s="226" t="str">
+      <c r="E12" s="213" t="str">
         <f t="shared" si="3"/>
         <v>Tranchant</v>
       </c>
-      <c r="F12" s="227" t="s">
+      <c r="F12" s="214" t="s">
         <v>33</v>
       </c>
       <c r="G12" s="14" t="s">
@@ -78063,16 +78062,16 @@
       </c>
     </row>
     <row r="13" spans="1:13" ht="15" customHeight="1">
-      <c r="A13" s="220" t="s">
+      <c r="A13" s="223" t="s">
         <v>57</v>
       </c>
-      <c r="B13" s="221"/>
-      <c r="C13" s="221"/>
-      <c r="D13" s="221"/>
-      <c r="E13" s="221"/>
-      <c r="F13" s="221"/>
-      <c r="G13" s="221"/>
-      <c r="H13" s="222"/>
+      <c r="B13" s="224"/>
+      <c r="C13" s="224"/>
+      <c r="D13" s="224"/>
+      <c r="E13" s="224"/>
+      <c r="F13" s="224"/>
+      <c r="G13" s="224"/>
+      <c r="H13" s="225"/>
       <c r="I13" s="116"/>
       <c r="J13" s="116"/>
       <c r="K13" s="119"/>
@@ -78088,11 +78087,11 @@
       <c r="C14" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="D14" s="226" t="str">
+      <c r="D14" s="213" t="str">
         <f>LEFT(C14,FIND(" ",C14))</f>
         <v xml:space="preserve">1d8 </v>
       </c>
-      <c r="E14" s="226" t="str">
+      <c r="E14" s="213" t="str">
         <f>PROPER(RIGHT(C14,LEN(C14)-LEN(D14)))</f>
         <v>Perforant</v>
       </c>
@@ -78194,11 +78193,11 @@
       <c r="C16" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="226" t="str">
+      <c r="D16" s="213" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve">1d4 </v>
       </c>
-      <c r="E16" s="226" t="str">
+      <c r="E16" s="213" t="str">
         <f t="shared" si="6"/>
         <v>Perforant</v>
       </c>
@@ -78291,16 +78290,16 @@
       </c>
     </row>
     <row r="18" spans="1:13" ht="15" customHeight="1">
-      <c r="A18" s="220" t="s">
+      <c r="A18" s="223" t="s">
         <v>71</v>
       </c>
-      <c r="B18" s="221"/>
-      <c r="C18" s="221"/>
-      <c r="D18" s="221"/>
-      <c r="E18" s="221"/>
-      <c r="F18" s="221"/>
-      <c r="G18" s="221"/>
-      <c r="H18" s="222"/>
+      <c r="B18" s="224"/>
+      <c r="C18" s="224"/>
+      <c r="D18" s="224"/>
+      <c r="E18" s="224"/>
+      <c r="F18" s="224"/>
+      <c r="G18" s="224"/>
+      <c r="H18" s="225"/>
       <c r="I18" s="116"/>
       <c r="J18" s="116"/>
       <c r="K18" s="119"/>
@@ -78369,11 +78368,11 @@
       <c r="C20" s="36" t="s">
         <v>75</v>
       </c>
-      <c r="D20" s="226" t="str">
+      <c r="D20" s="213" t="str">
         <f t="shared" ref="D20:D36" si="9">LEFT(C20,FIND(" ",C20))</f>
         <v xml:space="preserve">1d10 </v>
       </c>
-      <c r="E20" s="226" t="str">
+      <c r="E20" s="213" t="str">
         <f t="shared" ref="E20:E36" si="10">PROPER(RIGHT(C20,LEN(C20)-LEN(D20)))</f>
         <v>Tranchant</v>
       </c>
@@ -78475,11 +78474,11 @@
       <c r="C22" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="D22" s="226" t="str">
+      <c r="D22" s="213" t="str">
         <f t="shared" si="9"/>
         <v xml:space="preserve">1d6 </v>
       </c>
-      <c r="E22" s="226" t="str">
+      <c r="E22" s="213" t="str">
         <f t="shared" si="10"/>
         <v>Perforant</v>
       </c>
@@ -78581,11 +78580,11 @@
       <c r="C24" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="D24" s="226" t="str">
+      <c r="D24" s="213" t="str">
         <f t="shared" si="9"/>
         <v xml:space="preserve">1d8 </v>
       </c>
-      <c r="E24" s="226" t="str">
+      <c r="E24" s="213" t="str">
         <f t="shared" si="10"/>
         <v>Contondant</v>
       </c>
@@ -78687,11 +78686,11 @@
       <c r="C26" s="36" t="s">
         <v>93</v>
       </c>
-      <c r="D26" s="226" t="str">
+      <c r="D26" s="213" t="str">
         <f t="shared" si="9"/>
         <v xml:space="preserve">1d12 </v>
       </c>
-      <c r="E26" s="226" t="str">
+      <c r="E26" s="213" t="str">
         <f t="shared" si="10"/>
         <v>Tranchant</v>
       </c>
@@ -78793,11 +78792,11 @@
       <c r="C28" s="36" t="s">
         <v>75</v>
       </c>
-      <c r="D28" s="226" t="str">
+      <c r="D28" s="213" t="str">
         <f t="shared" si="9"/>
         <v xml:space="preserve">1d10 </v>
       </c>
-      <c r="E28" s="226" t="str">
+      <c r="E28" s="213" t="str">
         <f t="shared" si="10"/>
         <v>Tranchant</v>
       </c>
@@ -78899,11 +78898,11 @@
       <c r="C30" s="36" t="s">
         <v>102</v>
       </c>
-      <c r="D30" s="226" t="str">
+      <c r="D30" s="213" t="str">
         <f t="shared" si="9"/>
         <v xml:space="preserve">2d6 </v>
       </c>
-      <c r="E30" s="226" t="str">
+      <c r="E30" s="213" t="str">
         <f t="shared" si="10"/>
         <v>Contondant</v>
       </c>
@@ -79005,11 +79004,11 @@
       <c r="C32" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="D32" s="226" t="str">
+      <c r="D32" s="213" t="str">
         <f t="shared" si="9"/>
         <v xml:space="preserve">1d8 </v>
       </c>
-      <c r="E32" s="226" t="str">
+      <c r="E32" s="213" t="str">
         <f t="shared" si="10"/>
         <v>Perforant</v>
       </c>
@@ -79111,11 +79110,11 @@
       <c r="C34" s="36" t="s">
         <v>107</v>
       </c>
-      <c r="D34" s="226" t="str">
+      <c r="D34" s="213" t="str">
         <f t="shared" si="9"/>
         <v xml:space="preserve">1d10 </v>
       </c>
-      <c r="E34" s="226" t="str">
+      <c r="E34" s="213" t="str">
         <f t="shared" si="10"/>
         <v>Perforant</v>
       </c>
@@ -79217,11 +79216,11 @@
       <c r="C36" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="D36" s="226" t="str">
+      <c r="D36" s="213" t="str">
         <f t="shared" si="9"/>
         <v xml:space="preserve">1d6 </v>
       </c>
-      <c r="E36" s="226" t="str">
+      <c r="E36" s="213" t="str">
         <f t="shared" si="10"/>
         <v>Perforant</v>
       </c>
@@ -79261,16 +79260,16 @@
       </c>
     </row>
     <row r="37" spans="1:13" ht="15" customHeight="1">
-      <c r="A37" s="220" t="s">
+      <c r="A37" s="223" t="s">
         <v>112</v>
       </c>
-      <c r="B37" s="221"/>
-      <c r="C37" s="221"/>
-      <c r="D37" s="221"/>
-      <c r="E37" s="221"/>
-      <c r="F37" s="221"/>
-      <c r="G37" s="221"/>
-      <c r="H37" s="222"/>
+      <c r="B37" s="224"/>
+      <c r="C37" s="224"/>
+      <c r="D37" s="224"/>
+      <c r="E37" s="224"/>
+      <c r="F37" s="224"/>
+      <c r="G37" s="224"/>
+      <c r="H37" s="225"/>
       <c r="I37" s="116"/>
       <c r="J37" s="116"/>
       <c r="K37" s="119"/>
@@ -79286,11 +79285,11 @@
       <c r="C38" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="D38" s="226" t="str">
+      <c r="D38" s="213" t="str">
         <f>LEFT(C38,FIND(" ",C38))</f>
         <v xml:space="preserve">1d6 </v>
       </c>
-      <c r="E38" s="226" t="str">
+      <c r="E38" s="213" t="str">
         <f>PROPER(RIGHT(C38,LEN(C38)-LEN(D38)))</f>
         <v>Perforant</v>
       </c>
@@ -79392,11 +79391,11 @@
       <c r="C40" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="D40" s="226" t="str">
+      <c r="D40" s="213" t="str">
         <f t="shared" si="11"/>
         <v xml:space="preserve">1d8 </v>
       </c>
-      <c r="E40" s="226" t="str">
+      <c r="E40" s="213" t="str">
         <f t="shared" si="12"/>
         <v>Perforant</v>
       </c>
@@ -79490,11 +79489,11 @@
       <c r="C42" s="39" t="s">
         <v>122</v>
       </c>
-      <c r="D42" s="225" t="str">
+      <c r="D42" s="212" t="str">
         <f t="shared" si="11"/>
         <v xml:space="preserve">1 </v>
       </c>
-      <c r="E42" s="225" t="str">
+      <c r="E42" s="212" t="str">
         <f t="shared" si="12"/>
         <v>Perforant</v>
       </c>
@@ -80004,17 +80003,17 @@
       </c>
     </row>
     <row r="2" spans="1:14" s="133" customFormat="1">
-      <c r="A2" s="223" t="s">
+      <c r="A2" s="226" t="s">
         <v>488</v>
       </c>
-      <c r="B2" s="223"/>
-      <c r="C2" s="223"/>
-      <c r="D2" s="223"/>
-      <c r="E2" s="223"/>
-      <c r="F2" s="223"/>
-      <c r="G2" s="223"/>
-      <c r="H2" s="223"/>
-      <c r="I2" s="223"/>
+      <c r="B2" s="226"/>
+      <c r="C2" s="226"/>
+      <c r="D2" s="226"/>
+      <c r="E2" s="226"/>
+      <c r="F2" s="226"/>
+      <c r="G2" s="226"/>
+      <c r="H2" s="226"/>
+      <c r="I2" s="226"/>
     </row>
     <row r="3" spans="1:14" ht="15" customHeight="1">
       <c r="A3" s="123" t="s">
@@ -80201,17 +80200,17 @@
       </c>
     </row>
     <row r="6" spans="1:14" s="133" customFormat="1">
-      <c r="A6" s="223" t="s">
+      <c r="A6" s="226" t="s">
         <v>499</v>
       </c>
-      <c r="B6" s="223"/>
-      <c r="C6" s="223"/>
-      <c r="D6" s="223"/>
-      <c r="E6" s="223"/>
-      <c r="F6" s="223"/>
-      <c r="G6" s="223"/>
-      <c r="H6" s="223"/>
-      <c r="I6" s="223"/>
+      <c r="B6" s="226"/>
+      <c r="C6" s="226"/>
+      <c r="D6" s="226"/>
+      <c r="E6" s="226"/>
+      <c r="F6" s="226"/>
+      <c r="G6" s="226"/>
+      <c r="H6" s="226"/>
+      <c r="I6" s="226"/>
       <c r="J6" s="130"/>
       <c r="L6" s="132"/>
       <c r="M6" s="132"/>
@@ -80498,17 +80497,17 @@
       </c>
     </row>
     <row r="12" spans="1:14" s="133" customFormat="1">
-      <c r="A12" s="223" t="s">
+      <c r="A12" s="226" t="s">
         <v>516</v>
       </c>
-      <c r="B12" s="223"/>
-      <c r="C12" s="223"/>
-      <c r="D12" s="223"/>
-      <c r="E12" s="223"/>
-      <c r="F12" s="223"/>
-      <c r="G12" s="223"/>
-      <c r="H12" s="223"/>
-      <c r="I12" s="223"/>
+      <c r="B12" s="226"/>
+      <c r="C12" s="226"/>
+      <c r="D12" s="226"/>
+      <c r="E12" s="226"/>
+      <c r="F12" s="226"/>
+      <c r="G12" s="226"/>
+      <c r="H12" s="226"/>
+      <c r="I12" s="226"/>
       <c r="J12" s="130"/>
       <c r="L12" s="132"/>
       <c r="M12" s="132"/>
@@ -80723,17 +80722,17 @@
       </c>
     </row>
     <row r="17" spans="1:14" s="133" customFormat="1">
-      <c r="A17" s="224" t="s">
+      <c r="A17" s="227" t="s">
         <v>530</v>
       </c>
-      <c r="B17" s="224"/>
-      <c r="C17" s="224"/>
-      <c r="D17" s="224"/>
-      <c r="E17" s="224"/>
-      <c r="F17" s="224"/>
-      <c r="G17" s="224"/>
-      <c r="H17" s="224"/>
-      <c r="I17" s="224"/>
+      <c r="B17" s="227"/>
+      <c r="C17" s="227"/>
+      <c r="D17" s="227"/>
+      <c r="E17" s="227"/>
+      <c r="F17" s="227"/>
+      <c r="G17" s="227"/>
+      <c r="H17" s="227"/>
+      <c r="I17" s="227"/>
       <c r="J17" s="130"/>
       <c r="K17" s="131"/>
       <c r="L17" s="132"/>

</xml_diff>

<commit_message>
Save advantages & alterations
</commit_message>
<xml_diff>
--- a/Donjons_et_dragons.xlsx
+++ b/Donjons_et_dragons.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7515" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7515" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Niveaux" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5629" uniqueCount="2924">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5629" uniqueCount="2925">
   <si>
     <t>Niveau</t>
   </si>
@@ -10196,6 +10196,9 @@
   </si>
   <si>
     <t>"CON", "CHA"</t>
+  </si>
+  <si>
+    <t>Avantages de sauvegardes</t>
   </si>
 </sst>
 </file>
@@ -11308,20 +11311,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="34" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="33" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="34" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="34" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="34" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -11347,8 +11352,6 @@
     <xf numFmtId="0" fontId="32" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -45561,7 +45564,7 @@
  "Charisma" : 0,
  "Speed" : 9,
  "Resistances" : [],
- "Saves" : ["Seduced"]
+ "SaveAdvantages" : ["Seduced"]
   },
 "HALFELIN": {
  "Id" : "HALFELIN",
@@ -45575,7 +45578,7 @@
  "Charisma" : 0,
  "Speed" : 7.5,
  "Resistances" : [],
- "Saves" : ["Scared"]
+ "SaveAdvantages" : ["Scared"]
   },
 "HUMAN": {
  "Id" : "HUMAN",
@@ -45589,7 +45592,7 @@
  "Charisma" : 1,
  "Speed" : 9,
  "Resistances" : [],
- "Saves" : []
+ "SaveAdvantages" : []
   },
 "DWARF": {
  "Id" : "DWARF",
@@ -45603,7 +45606,7 @@
  "Charisma" : 0,
  "Speed" : 7.5,
  "Resistances" : ["Poisonned"],
- "Saves" : ["Poisonned"]
+ "SaveAdvantages" : ["Poisonned"]
   },
 "HALF_ELF": {
  "Id" : "HALF_ELF",
@@ -45617,7 +45620,7 @@
  "Charisma" : 2,
  "Speed" : 9,
  "Resistances" : [],
- "Saves" : []
+ "SaveAdvantages" : []
   },
 "HALF_ORC": {
  "Id" : "HALF_ORC",
@@ -45631,7 +45634,7 @@
  "Charisma" : 0,
  "Speed" : 9,
  "Resistances" : [],
- "Saves" : []
+ "SaveAdvantages" : []
   },
 "DRAGON_BORN": {
  "Id" : "DRAGON_BORN",
@@ -45645,7 +45648,7 @@
  "Charisma" : 1,
  "Speed" : 9,
  "Resistances" : [],
- "Saves" : []
+ "SaveAdvantages" : []
   },
 "GNOME": {
  "Id" : "GNOME",
@@ -45659,7 +45662,7 @@
  "Charisma" : 0,
  "Speed" : 7.5,
  "Resistances" : [],
- "Saves" : ["Intelligence", "Wisdom", "Charisma"]
+ "SaveAdvantages" : ["Intelligence", "Wisdom", "Charisma"]
   },
 "TIEFFLING": {
  "Id" : "TIEFFLING",
@@ -45673,7 +45676,7 @@
  "Charisma" : 2,
  "Speed" : 9,
  "Resistances" : [],
- "Saves" : []
+ "SaveAdvantages" : []
   },
 "AARAKOCRA": {
  "Id" : "AARAKOCRA",
@@ -45687,7 +45690,7 @@
  "Charisma" : 0,
  "Speed" : 7.5,
  "Resistances" : [],
- "Saves" : []
+ "SaveAdvantages" : []
   },
 "GENASI": {
  "Id" : "GENASI",
@@ -45701,7 +45704,7 @@
  "Charisma" : 0,
  "Speed" : 9,
  "Resistances" : [],
- "Saves" : []
+ "SaveAdvantages" : []
   },
 "GOLIATH": {
  "Id" : "GOLIATH",
@@ -45715,7 +45718,7 @@
  "Charisma" : 0,
  "Speed" : 9,
  "Resistances" : [],
- "Saves" : []
+ "SaveAdvantages" : []
   }</v>
       </c>
       <c r="C1" t="str">
@@ -45735,7 +45738,7 @@
  "Charisma" : 0,
  "Speed" : 9,
  "Resistances" : [],
- "Saves" : ["Seduced"]
+ "SaveAdvantages" : ["Seduced"]
   },
 "HALFELIN": {
  "Id" : "HALFELIN",
@@ -45749,7 +45752,7 @@
  "Charisma" : 0,
  "Speed" : 7.5,
  "Resistances" : [],
- "Saves" : ["Scared"]
+ "SaveAdvantages" : ["Scared"]
   },
 "HUMAN": {
  "Id" : "HUMAN",
@@ -45763,7 +45766,7 @@
  "Charisma" : 1,
  "Speed" : 9,
  "Resistances" : [],
- "Saves" : []
+ "SaveAdvantages" : []
   },
 "DWARF": {
  "Id" : "DWARF",
@@ -45777,7 +45780,7 @@
  "Charisma" : 0,
  "Speed" : 7.5,
  "Resistances" : ["Poisonned"],
- "Saves" : ["Poisonned"]
+ "SaveAdvantages" : ["Poisonned"]
   },
 "HALF_ELF": {
  "Id" : "HALF_ELF",
@@ -45791,7 +45794,7 @@
  "Charisma" : 2,
  "Speed" : 9,
  "Resistances" : [],
- "Saves" : []
+ "SaveAdvantages" : []
   },
 "HALF_ORC": {
  "Id" : "HALF_ORC",
@@ -45805,7 +45808,7 @@
  "Charisma" : 0,
  "Speed" : 9,
  "Resistances" : [],
- "Saves" : []
+ "SaveAdvantages" : []
   },
 "DRAGON_BORN": {
  "Id" : "DRAGON_BORN",
@@ -45819,7 +45822,7 @@
  "Charisma" : 1,
  "Speed" : 9,
  "Resistances" : [],
- "Saves" : []
+ "SaveAdvantages" : []
   },
 "GNOME": {
  "Id" : "GNOME",
@@ -45833,7 +45836,7 @@
  "Charisma" : 0,
  "Speed" : 7.5,
  "Resistances" : [],
- "Saves" : ["Intelligence", "Wisdom", "Charisma"]
+ "SaveAdvantages" : ["Intelligence", "Wisdom", "Charisma"]
   },
 "TIEFFLING": {
  "Id" : "TIEFFLING",
@@ -45847,7 +45850,7 @@
  "Charisma" : 2,
  "Speed" : 9,
  "Resistances" : [],
- "Saves" : []
+ "SaveAdvantages" : []
   },
 "AARAKOCRA": {
  "Id" : "AARAKOCRA",
@@ -45861,7 +45864,7 @@
  "Charisma" : 0,
  "Speed" : 7.5,
  "Resistances" : [],
- "Saves" : []
+ "SaveAdvantages" : []
   },
 "GENASI": {
  "Id" : "GENASI",
@@ -45875,7 +45878,7 @@
  "Charisma" : 0,
  "Speed" : 9,
  "Resistances" : [],
- "Saves" : []
+ "SaveAdvantages" : []
   },
 "GOLIATH": {
  "Id" : "GOLIATH",
@@ -45889,7 +45892,7 @@
  "Charisma" : 0,
  "Speed" : 9,
  "Resistances" : [],
- "Saves" : []
+ "SaveAdvantages" : []
   }
  }</v>
       </c>
@@ -45913,7 +45916,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : [],
- "Saves" : [],
+ "SaveAdvantages" : [],
  "ArmorCategories" : []
   },
 "WOODEN_ELF": {
@@ -45929,7 +45932,7 @@
  "Charisma" : 0,
  "Speed" : 10.5,
  "Resistances" : [],
- "Saves" : [],
+ "SaveAdvantages" : [],
  "ArmorCategories" : []
   },
 "DROW": {
@@ -45945,7 +45948,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : [],
- "Saves" : [],
+ "SaveAdvantages" : [],
  "ArmorCategories" : []
   },
 "LIGHT_FOOT_HALFELIN": {
@@ -45961,7 +45964,7 @@
  "Charisma" : 1,
  "Speed" : 0,
  "Resistances" : [],
- "Saves" : [],
+ "SaveAdvantages" : [],
  "ArmorCategories" : []
   },
 "ROBUST_HALFELIN": {
@@ -45977,7 +45980,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : ["Poisonned"],
- "Saves" : ["Poisonned"],
+ "SaveAdvantages" : ["Poisonned"],
  "ArmorCategories" : []
   },
 "HILLS_DWARF": {
@@ -45993,7 +45996,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : [],
- "Saves" : [],
+ "SaveAdvantages" : [],
  "ArmorCategories" : []
   },
 "MONTAINS_DWARF": {
@@ -46009,7 +46012,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : [],
- "Saves" : [],
+ "SaveAdvantages" : [],
  "ArmorCategories" : ["1_LIGHT", "2_MID"]
   },
 "FORESTS_GNOME": {
@@ -46025,7 +46028,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : [],
- "Saves" : [],
+ "SaveAdvantages" : [],
  "ArmorCategories" : []
   },
 "ROCKS_GNOME": {
@@ -46041,7 +46044,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : [],
- "Saves" : [],
+ "SaveAdvantages" : [],
  "ArmorCategories" : []
   },
 "DEPTH_GNOME": {
@@ -46057,7 +46060,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : [],
- "Saves" : [],
+ "SaveAdvantages" : [],
  "ArmorCategories" : []
   },
 "AIR_GENASI": {
@@ -46073,7 +46076,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : [],
- "Saves" : [],
+ "SaveAdvantages" : [],
  "ArmorCategories" : []
   },
 "EARTH_GENASI": {
@@ -46089,7 +46092,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : [],
- "Saves" : [],
+ "SaveAdvantages" : [],
  "ArmorCategories" : []
   },
 "FIRE_GENASI": {
@@ -46105,7 +46108,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : ["Burned"],
- "Saves" : ["Burned"],
+ "SaveAdvantages" : ["Burned"],
  "ArmorCategories" : []
   },
 "WATER_GENASI": {
@@ -46121,7 +46124,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : ["Acidified"],
- "Saves" : ["Acidified"],
+ "SaveAdvantages" : ["Acidified"],
  "ArmorCategories" : []
   },
 "HUMAN": {
@@ -46137,7 +46140,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : [],
- "Saves" : [],
+ "SaveAdvantages" : [],
  "ArmorCategories" : []
   },
 "HALF_ELF": {
@@ -46153,7 +46156,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : [],
- "Saves" : [],
+ "SaveAdvantages" : [],
  "ArmorCategories" : []
   },
 "HALF_ORC": {
@@ -46169,7 +46172,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : [],
- "Saves" : [],
+ "SaveAdvantages" : [],
  "ArmorCategories" : []
   },
 "WHITE_DRAGON": {
@@ -46185,7 +46188,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : ["Cold"],
- "Saves" : ["Cold"],
+ "SaveAdvantages" : ["Cold"],
  "ArmorCategories" : []
   },
 "BLUE_DRAGON": {
@@ -46201,7 +46204,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : ["Electrified"],
- "Saves" : ["Electrified"],
+ "SaveAdvantages" : ["Electrified"],
  "ArmorCategories" : []
   },
 "BLACK_DRAGON": {
@@ -46217,7 +46220,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : ["Acidified"],
- "Saves" : ["Acidified"],
+ "SaveAdvantages" : ["Acidified"],
  "ArmorCategories" : []
   },
 "RED_DRAGON": {
@@ -46233,7 +46236,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : ["Burned"],
- "Saves" : ["Burned"],
+ "SaveAdvantages" : ["Burned"],
  "ArmorCategories" : []
   },
 "GREEN_DRAGON": {
@@ -46249,7 +46252,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : ["Poisonned"],
- "Saves" : ["Poisonned"],
+ "SaveAdvantages" : ["Poisonned"],
  "ArmorCategories" : []
   },
 "BRASS_DRAGON": {
@@ -46265,7 +46268,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : ["Burned"],
- "Saves" : ["Burned"],
+ "SaveAdvantages" : ["Burned"],
  "ArmorCategories" : []
   },
 "SILVER_DRAGON": {
@@ -46281,7 +46284,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : ["Cold"],
- "Saves" : ["Cold"],
+ "SaveAdvantages" : ["Cold"],
  "ArmorCategories" : []
   },
 "BRONZE_DRAGON": {
@@ -46297,7 +46300,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : ["Electrified"],
- "Saves" : ["Electrified"],
+ "SaveAdvantages" : ["Electrified"],
  "ArmorCategories" : []
   },
 "COPPER_DRAGON": {
@@ -46313,7 +46316,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : ["Acidified"],
- "Saves" : ["Acidified"],
+ "SaveAdvantages" : ["Acidified"],
  "ArmorCategories" : []
   },
 "GOLD_DRAGON": {
@@ -46329,7 +46332,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : ["Burned"],
- "Saves" : ["Burned"],
+ "SaveAdvantages" : ["Burned"],
  "ArmorCategories" : []
   },
 "TIEFFLING": {
@@ -46345,7 +46348,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : ["Burned"],
- "Saves" : ["Burned"],
+ "SaveAdvantages" : ["Burned"],
  "ArmorCategories" : []
   },
 "AARAKOCRA": {
@@ -46361,7 +46364,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : [],
- "Saves" : [],
+ "SaveAdvantages" : [],
  "ArmorCategories" : []
   },
 "GOLIATH": {
@@ -46377,7 +46380,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : [],
- "Saves" : [],
+ "SaveAdvantages" : [],
  "ArmorCategories" : []
   }</v>
       </c>
@@ -46399,7 +46402,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : [],
- "Saves" : [],
+ "SaveAdvantages" : [],
  "ArmorCategories" : []
   },
 "WOODEN_ELF": {
@@ -46415,7 +46418,7 @@
  "Charisma" : 0,
  "Speed" : 10.5,
  "Resistances" : [],
- "Saves" : [],
+ "SaveAdvantages" : [],
  "ArmorCategories" : []
   },
 "DROW": {
@@ -46431,7 +46434,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : [],
- "Saves" : [],
+ "SaveAdvantages" : [],
  "ArmorCategories" : []
   },
 "LIGHT_FOOT_HALFELIN": {
@@ -46447,7 +46450,7 @@
  "Charisma" : 1,
  "Speed" : 0,
  "Resistances" : [],
- "Saves" : [],
+ "SaveAdvantages" : [],
  "ArmorCategories" : []
   },
 "ROBUST_HALFELIN": {
@@ -46463,7 +46466,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : ["Poisonned"],
- "Saves" : ["Poisonned"],
+ "SaveAdvantages" : ["Poisonned"],
  "ArmorCategories" : []
   },
 "HILLS_DWARF": {
@@ -46479,7 +46482,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : [],
- "Saves" : [],
+ "SaveAdvantages" : [],
  "ArmorCategories" : []
   },
 "MONTAINS_DWARF": {
@@ -46495,7 +46498,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : [],
- "Saves" : [],
+ "SaveAdvantages" : [],
  "ArmorCategories" : ["1_LIGHT", "2_MID"]
   },
 "FORESTS_GNOME": {
@@ -46511,7 +46514,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : [],
- "Saves" : [],
+ "SaveAdvantages" : [],
  "ArmorCategories" : []
   },
 "ROCKS_GNOME": {
@@ -46527,7 +46530,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : [],
- "Saves" : [],
+ "SaveAdvantages" : [],
  "ArmorCategories" : []
   },
 "DEPTH_GNOME": {
@@ -46543,7 +46546,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : [],
- "Saves" : [],
+ "SaveAdvantages" : [],
  "ArmorCategories" : []
   },
 "AIR_GENASI": {
@@ -46559,7 +46562,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : [],
- "Saves" : [],
+ "SaveAdvantages" : [],
  "ArmorCategories" : []
   },
 "EARTH_GENASI": {
@@ -46575,7 +46578,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : [],
- "Saves" : [],
+ "SaveAdvantages" : [],
  "ArmorCategories" : []
   },
 "FIRE_GENASI": {
@@ -46591,7 +46594,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : ["Burned"],
- "Saves" : ["Burned"],
+ "SaveAdvantages" : ["Burned"],
  "ArmorCategories" : []
   },
 "WATER_GENASI": {
@@ -46607,7 +46610,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : ["Acidified"],
- "Saves" : ["Acidified"],
+ "SaveAdvantages" : ["Acidified"],
  "ArmorCategories" : []
   },
 "HUMAN": {
@@ -46623,7 +46626,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : [],
- "Saves" : [],
+ "SaveAdvantages" : [],
  "ArmorCategories" : []
   },
 "HALF_ELF": {
@@ -46639,7 +46642,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : [],
- "Saves" : [],
+ "SaveAdvantages" : [],
  "ArmorCategories" : []
   },
 "HALF_ORC": {
@@ -46655,7 +46658,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : [],
- "Saves" : [],
+ "SaveAdvantages" : [],
  "ArmorCategories" : []
   },
 "WHITE_DRAGON": {
@@ -46671,7 +46674,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : ["Cold"],
- "Saves" : ["Cold"],
+ "SaveAdvantages" : ["Cold"],
  "ArmorCategories" : []
   },
 "BLUE_DRAGON": {
@@ -46687,7 +46690,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : ["Electrified"],
- "Saves" : ["Electrified"],
+ "SaveAdvantages" : ["Electrified"],
  "ArmorCategories" : []
   },
 "BLACK_DRAGON": {
@@ -46703,7 +46706,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : ["Acidified"],
- "Saves" : ["Acidified"],
+ "SaveAdvantages" : ["Acidified"],
  "ArmorCategories" : []
   },
 "RED_DRAGON": {
@@ -46719,7 +46722,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : ["Burned"],
- "Saves" : ["Burned"],
+ "SaveAdvantages" : ["Burned"],
  "ArmorCategories" : []
   },
 "GREEN_DRAGON": {
@@ -46735,7 +46738,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : ["Poisonned"],
- "Saves" : ["Poisonned"],
+ "SaveAdvantages" : ["Poisonned"],
  "ArmorCategories" : []
   },
 "BRASS_DRAGON": {
@@ -46751,7 +46754,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : ["Burned"],
- "Saves" : ["Burned"],
+ "SaveAdvantages" : ["Burned"],
  "ArmorCategories" : []
   },
 "SILVER_DRAGON": {
@@ -46767,7 +46770,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : ["Cold"],
- "Saves" : ["Cold"],
+ "SaveAdvantages" : ["Cold"],
  "ArmorCategories" : []
   },
 "BRONZE_DRAGON": {
@@ -46783,7 +46786,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : ["Electrified"],
- "Saves" : ["Electrified"],
+ "SaveAdvantages" : ["Electrified"],
  "ArmorCategories" : []
   },
 "COPPER_DRAGON": {
@@ -46799,7 +46802,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : ["Acidified"],
- "Saves" : ["Acidified"],
+ "SaveAdvantages" : ["Acidified"],
  "ArmorCategories" : []
   },
 "GOLD_DRAGON": {
@@ -46815,7 +46818,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : ["Burned"],
- "Saves" : ["Burned"],
+ "SaveAdvantages" : ["Burned"],
  "ArmorCategories" : []
   },
 "TIEFFLING": {
@@ -46831,7 +46834,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : ["Burned"],
- "Saves" : ["Burned"],
+ "SaveAdvantages" : ["Burned"],
  "ArmorCategories" : []
   },
 "AARAKOCRA": {
@@ -46847,7 +46850,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : [],
- "Saves" : [],
+ "SaveAdvantages" : [],
  "ArmorCategories" : []
   },
 "GOLIATH": {
@@ -46863,7 +46866,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : [],
- "Saves" : [],
+ "SaveAdvantages" : [],
  "ArmorCategories" : []
   }
  }</v>
@@ -57737,7 +57740,7 @@
 ",C26,",
 ",C27)&amp;"
 }"</f>
-        <v>{
+        <v xml:space="preserve">{
 " Races" : {
  "ELF": {
  "Id" : "ELF",
@@ -57751,7 +57754,7 @@
  "Charisma" : 0,
  "Speed" : 9,
  "Resistances" : [],
- "Saves" : ["Seduced"]
+ "SaveAdvantages" : ["Seduced"]
   },
 "HALFELIN": {
  "Id" : "HALFELIN",
@@ -57765,7 +57768,7 @@
  "Charisma" : 0,
  "Speed" : 7.5,
  "Resistances" : [],
- "Saves" : ["Scared"]
+ "SaveAdvantages" : ["Scared"]
   },
 "HUMAN": {
  "Id" : "HUMAN",
@@ -57779,7 +57782,7 @@
  "Charisma" : 1,
  "Speed" : 9,
  "Resistances" : [],
- "Saves" : []
+ "SaveAdvantages" : []
   },
 "DWARF": {
  "Id" : "DWARF",
@@ -57793,7 +57796,7 @@
  "Charisma" : 0,
  "Speed" : 7.5,
  "Resistances" : ["Poisonned"],
- "Saves" : ["Poisonned"]
+ "SaveAdvantages" : ["Poisonned"]
   },
 "HALF_ELF": {
  "Id" : "HALF_ELF",
@@ -57807,7 +57810,7 @@
  "Charisma" : 2,
  "Speed" : 9,
  "Resistances" : [],
- "Saves" : []
+ "SaveAdvantages" : []
   },
 "HALF_ORC": {
  "Id" : "HALF_ORC",
@@ -57821,7 +57824,7 @@
  "Charisma" : 0,
  "Speed" : 9,
  "Resistances" : [],
- "Saves" : []
+ "SaveAdvantages" : []
   },
 "DRAGON_BORN": {
  "Id" : "DRAGON_BORN",
@@ -57835,7 +57838,7 @@
  "Charisma" : 1,
  "Speed" : 9,
  "Resistances" : [],
- "Saves" : []
+ "SaveAdvantages" : []
   },
 "GNOME": {
  "Id" : "GNOME",
@@ -57849,7 +57852,7 @@
  "Charisma" : 0,
  "Speed" : 7.5,
  "Resistances" : [],
- "Saves" : ["Intelligence", "Wisdom", "Charisma"]
+ "SaveAdvantages" : ["Intelligence", "Wisdom", "Charisma"]
   },
 "TIEFFLING": {
  "Id" : "TIEFFLING",
@@ -57863,7 +57866,7 @@
  "Charisma" : 2,
  "Speed" : 9,
  "Resistances" : [],
- "Saves" : []
+ "SaveAdvantages" : []
   },
 "AARAKOCRA": {
  "Id" : "AARAKOCRA",
@@ -57877,7 +57880,7 @@
  "Charisma" : 0,
  "Speed" : 7.5,
  "Resistances" : [],
- "Saves" : []
+ "SaveAdvantages" : []
   },
 "GENASI": {
  "Id" : "GENASI",
@@ -57891,7 +57894,7 @@
  "Charisma" : 0,
  "Speed" : 9,
  "Resistances" : [],
- "Saves" : []
+ "SaveAdvantages" : []
   },
 "GOLIATH": {
  "Id" : "GOLIATH",
@@ -57905,7 +57908,7 @@
  "Charisma" : 0,
  "Speed" : 9,
  "Resistances" : [],
- "Saves" : []
+ "SaveAdvantages" : []
   }
  },
 "SubRaces" : {
@@ -57922,7 +57925,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : [],
- "Saves" : [],
+ "SaveAdvantages" : [],
  "ArmorCategories" : []
   },
 "WOODEN_ELF": {
@@ -57938,7 +57941,7 @@
  "Charisma" : 0,
  "Speed" : 10.5,
  "Resistances" : [],
- "Saves" : [],
+ "SaveAdvantages" : [],
  "ArmorCategories" : []
   },
 "DROW": {
@@ -57954,7 +57957,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : [],
- "Saves" : [],
+ "SaveAdvantages" : [],
  "ArmorCategories" : []
   },
 "LIGHT_FOOT_HALFELIN": {
@@ -57970,7 +57973,7 @@
  "Charisma" : 1,
  "Speed" : 0,
  "Resistances" : [],
- "Saves" : [],
+ "SaveAdvantages" : [],
  "ArmorCategories" : []
   },
 "ROBUST_HALFELIN": {
@@ -57986,7 +57989,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : ["Poisonned"],
- "Saves" : ["Poisonned"],
+ "SaveAdvantages" : ["Poisonned"],
  "ArmorCategories" : []
   },
 "HILLS_DWARF": {
@@ -58002,7 +58005,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : [],
- "Saves" : [],
+ "SaveAdvantages" : [],
  "ArmorCategories" : []
   },
 "MONTAINS_DWARF": {
@@ -58018,7 +58021,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : [],
- "Saves" : [],
+ "SaveAdvantages" : [],
  "ArmorCategories" : ["1_LIGHT", "2_MID"]
   },
 "FORESTS_GNOME": {
@@ -58034,7 +58037,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : [],
- "Saves" : [],
+ "SaveAdvantages" : [],
  "ArmorCategories" : []
   },
 "ROCKS_GNOME": {
@@ -58050,7 +58053,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : [],
- "Saves" : [],
+ "SaveAdvantages" : [],
  "ArmorCategories" : []
   },
 "DEPTH_GNOME": {
@@ -58066,7 +58069,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : [],
- "Saves" : [],
+ "SaveAdvantages" : [],
  "ArmorCategories" : []
   },
 "AIR_GENASI": {
@@ -58082,7 +58085,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : [],
- "Saves" : [],
+ "SaveAdvantages" : [],
  "ArmorCategories" : []
   },
 "EARTH_GENASI": {
@@ -58098,7 +58101,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : [],
- "Saves" : [],
+ "SaveAdvantages" : [],
  "ArmorCategories" : []
   },
 "FIRE_GENASI": {
@@ -58114,7 +58117,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : ["Burned"],
- "Saves" : ["Burned"],
+ "SaveAdvantages" : ["Burned"],
  "ArmorCategories" : []
   },
 "WATER_GENASI": {
@@ -58130,7 +58133,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : ["Acidified"],
- "Saves" : ["Acidified"],
+ "SaveAdvantages" : ["Acidified"],
  "ArmorCategories" : []
   },
 "HUMAN": {
@@ -58146,7 +58149,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : [],
- "Saves" : [],
+ "SaveAdvantages" : [],
  "ArmorCategories" : []
   },
 "HALF_ELF": {
@@ -58162,7 +58165,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : [],
- "Saves" : [],
+ "SaveAdvantages" : [],
  "ArmorCategories" : []
   },
 "HALF_ORC": {
@@ -58178,7 +58181,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : [],
- "Saves" : [],
+ "SaveAdvantages" : [],
  "ArmorCategories" : []
   },
 "WHITE_DRAGON": {
@@ -58194,7 +58197,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : ["Cold"],
- "Saves" : ["Cold"],
+ "SaveAdvantages" : ["Cold"],
  "ArmorCategories" : []
   },
 "BLUE_DRAGON": {
@@ -58210,7 +58213,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : ["Electrified"],
- "Saves" : ["Electrified"],
+ "SaveAdvantages" : ["Electrified"],
  "ArmorCategories" : []
   },
 "BLACK_DRAGON": {
@@ -58226,7 +58229,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : ["Acidified"],
- "Saves" : ["Acidified"],
+ "SaveAdvantages" : ["Acidified"],
  "ArmorCategories" : []
   },
 "RED_DRAGON": {
@@ -58242,7 +58245,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : ["Burned"],
- "Saves" : ["Burned"],
+ "SaveAdvantages" : ["Burned"],
  "ArmorCategories" : []
   },
 "GREEN_DRAGON": {
@@ -58258,7 +58261,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : ["Poisonned"],
- "Saves" : ["Poisonned"],
+ "SaveAdvantages" : ["Poisonned"],
  "ArmorCategories" : []
   },
 "BRASS_DRAGON": {
@@ -58274,7 +58277,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : ["Burned"],
- "Saves" : ["Burned"],
+ "SaveAdvantages" : ["Burned"],
  "ArmorCategories" : []
   },
 "SILVER_DRAGON": {
@@ -58290,7 +58293,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : ["Cold"],
- "Saves" : ["Cold"],
+ "SaveAdvantages" : ["Cold"],
  "ArmorCategories" : []
   },
 "BRONZE_DRAGON": {
@@ -58306,7 +58309,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : ["Electrified"],
- "Saves" : ["Electrified"],
+ "SaveAdvantages" : ["Electrified"],
  "ArmorCategories" : []
   },
 "COPPER_DRAGON": {
@@ -58322,7 +58325,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : ["Acidified"],
- "Saves" : ["Acidified"],
+ "SaveAdvantages" : ["Acidified"],
  "ArmorCategories" : []
   },
 "GOLD_DRAGON": {
@@ -58338,7 +58341,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : ["Burned"],
- "Saves" : ["Burned"],
+ "SaveAdvantages" : ["Burned"],
  "ArmorCategories" : []
   },
 "TIEFFLING": {
@@ -58354,7 +58357,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : ["Burned"],
- "Saves" : ["Burned"],
+ "SaveAdvantages" : ["Burned"],
  "ArmorCategories" : []
   },
 "AARAKOCRA": {
@@ -58370,7 +58373,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : [],
- "Saves" : [],
+ "SaveAdvantages" : [],
  "ArmorCategories" : []
   },
 "GOLIATH": {
@@ -58386,7 +58389,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : [],
- "Saves" : [],
+ "SaveAdvantages" : [],
  "ArmorCategories" : []
   }
  },
@@ -59292,31 +59295,7 @@
  "Name" : "Tambour",
  "OV" : "  Drum",
  "Category": "MUSIC",
- "Weight" : 1500,
- "Price" : 600
-  },,
-"Tympanon": {
- "Name" : "Tympanon",
- "OV" : "  Dulcimer",
- "Category": "MUSIC",
- "Weight" : 5000,
- "Price" : 2500
-  },,
-"Viole": {
- "Name" : "Viole",
- "OV" : "  Viol",
- "Category": "MUSIC",
- "Weight" : 500,
- "Price" : 3000
-  },,
-"Dés": {
- "Name" : "Dés",
- "OV" : "  Dice set",
- "Category": "GAME",
- "Weight" : 0,
- "Price" : 10
-  },,
-"Jeu d'échecs drac</v>
+ "Weight" : </v>
       </c>
     </row>
   </sheetData>
@@ -59329,7 +59308,7 @@
   <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+      <selection activeCell="N2" sqref="N2:N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -59381,7 +59360,7 @@
         <v>2873</v>
       </c>
       <c r="L1" s="188" t="s">
-        <v>2877</v>
+        <v>2924</v>
       </c>
     </row>
     <row r="2" spans="1:14">
@@ -59432,7 +59411,7 @@
  ""Charisma"" : "&amp;I2&amp;",
  ""Speed"" : "&amp;SUBSTITUTE(J2,",",".")&amp;",
  ""Resistances"" : ["&amp;K2&amp;"],
- ""Saves"" : ["&amp;L2&amp;"]
+ ""SaveAdvantages"" : ["&amp;L2&amp;"]
   }"</f>
         <v>"ELF": {
  "Id" : "ELF",
@@ -59446,7 +59425,7 @@
  "Charisma" : 0,
  "Speed" : 9,
  "Resistances" : [],
- "Saves" : ["Seduced"]
+ "SaveAdvantages" : ["Seduced"]
   }</v>
       </c>
     </row>
@@ -59498,7 +59477,7 @@
  ""Charisma"" : "&amp;I3&amp;",
  ""Speed"" : "&amp;SUBSTITUTE(J3,",",".")&amp;",
  ""Resistances"" : ["&amp;K3&amp;"],
- ""Saves"" : ["&amp;L3&amp;"]
+ ""SaveAdvantages"" : ["&amp;L3&amp;"]
   }"</f>
         <v>"HALFELIN": {
  "Id" : "HALFELIN",
@@ -59512,7 +59491,7 @@
  "Charisma" : 0,
  "Speed" : 7.5,
  "Resistances" : [],
- "Saves" : ["Scared"]
+ "SaveAdvantages" : ["Scared"]
   }</v>
       </c>
     </row>
@@ -59563,7 +59542,7 @@
  "Charisma" : 1,
  "Speed" : 9,
  "Resistances" : [],
- "Saves" : []
+ "SaveAdvantages" : []
   }</v>
       </c>
     </row>
@@ -59618,7 +59597,7 @@
  "Charisma" : 0,
  "Speed" : 7.5,
  "Resistances" : ["Poisonned"],
- "Saves" : ["Poisonned"]
+ "SaveAdvantages" : ["Poisonned"]
   }</v>
       </c>
     </row>
@@ -59669,7 +59648,7 @@
  "Charisma" : 2,
  "Speed" : 9,
  "Resistances" : [],
- "Saves" : []
+ "SaveAdvantages" : []
   }</v>
       </c>
     </row>
@@ -59720,7 +59699,7 @@
  "Charisma" : 0,
  "Speed" : 9,
  "Resistances" : [],
- "Saves" : []
+ "SaveAdvantages" : []
   }</v>
       </c>
     </row>
@@ -59771,7 +59750,7 @@
  "Charisma" : 1,
  "Speed" : 9,
  "Resistances" : [],
- "Saves" : []
+ "SaveAdvantages" : []
   }</v>
       </c>
     </row>
@@ -59824,7 +59803,7 @@
  "Charisma" : 0,
  "Speed" : 7.5,
  "Resistances" : [],
- "Saves" : ["Intelligence", "Wisdom", "Charisma"]
+ "SaveAdvantages" : ["Intelligence", "Wisdom", "Charisma"]
   }</v>
       </c>
     </row>
@@ -59875,7 +59854,7 @@
  "Charisma" : 2,
  "Speed" : 9,
  "Resistances" : [],
- "Saves" : []
+ "SaveAdvantages" : []
   }</v>
       </c>
     </row>
@@ -59926,7 +59905,7 @@
  "Charisma" : 0,
  "Speed" : 7.5,
  "Resistances" : [],
- "Saves" : []
+ "SaveAdvantages" : []
   }</v>
       </c>
     </row>
@@ -59977,7 +59956,7 @@
  "Charisma" : 0,
  "Speed" : 9,
  "Resistances" : [],
- "Saves" : []
+ "SaveAdvantages" : []
   }</v>
       </c>
     </row>
@@ -60028,7 +60007,7 @@
  "Charisma" : 0,
  "Speed" : 9,
  "Resistances" : [],
- "Saves" : []
+ "SaveAdvantages" : []
   }</v>
       </c>
     </row>
@@ -60058,7 +60037,7 @@
  "Charisma" : 0,
  "Speed" : 9,
  "Resistances" : [],
- "Saves" : ["Seduced"]
+ "SaveAdvantages" : ["Seduced"]
   },
 "HALFELIN": {
  "Id" : "HALFELIN",
@@ -60072,7 +60051,7 @@
  "Charisma" : 0,
  "Speed" : 7.5,
  "Resistances" : [],
- "Saves" : ["Scared"]
+ "SaveAdvantages" : ["Scared"]
   },
 "HUMAN": {
  "Id" : "HUMAN",
@@ -60086,7 +60065,7 @@
  "Charisma" : 1,
  "Speed" : 9,
  "Resistances" : [],
- "Saves" : []
+ "SaveAdvantages" : []
   },
 "DWARF": {
  "Id" : "DWARF",
@@ -60100,7 +60079,7 @@
  "Charisma" : 0,
  "Speed" : 7.5,
  "Resistances" : ["Poisonned"],
- "Saves" : ["Poisonned"]
+ "SaveAdvantages" : ["Poisonned"]
   },
 "HALF_ELF": {
  "Id" : "HALF_ELF",
@@ -60114,7 +60093,7 @@
  "Charisma" : 2,
  "Speed" : 9,
  "Resistances" : [],
- "Saves" : []
+ "SaveAdvantages" : []
   },
 "HALF_ORC": {
  "Id" : "HALF_ORC",
@@ -60128,7 +60107,7 @@
  "Charisma" : 0,
  "Speed" : 9,
  "Resistances" : [],
- "Saves" : []
+ "SaveAdvantages" : []
   },
 "DRAGON_BORN": {
  "Id" : "DRAGON_BORN",
@@ -60142,7 +60121,7 @@
  "Charisma" : 1,
  "Speed" : 9,
  "Resistances" : [],
- "Saves" : []
+ "SaveAdvantages" : []
   },
 "GNOME": {
  "Id" : "GNOME",
@@ -60156,7 +60135,7 @@
  "Charisma" : 0,
  "Speed" : 7.5,
  "Resistances" : [],
- "Saves" : ["Intelligence", "Wisdom", "Charisma"]
+ "SaveAdvantages" : ["Intelligence", "Wisdom", "Charisma"]
   },
 "TIEFFLING": {
  "Id" : "TIEFFLING",
@@ -60170,7 +60149,7 @@
  "Charisma" : 2,
  "Speed" : 9,
  "Resistances" : [],
- "Saves" : []
+ "SaveAdvantages" : []
   },
 "AARAKOCRA": {
  "Id" : "AARAKOCRA",
@@ -60184,7 +60163,7 @@
  "Charisma" : 0,
  "Speed" : 7.5,
  "Resistances" : [],
- "Saves" : []
+ "SaveAdvantages" : []
   },
 "GENASI": {
  "Id" : "GENASI",
@@ -60198,7 +60177,7 @@
  "Charisma" : 0,
  "Speed" : 9,
  "Resistances" : [],
- "Saves" : []
+ "SaveAdvantages" : []
   },
 "GOLIATH": {
  "Id" : "GOLIATH",
@@ -60212,7 +60191,7 @@
  "Charisma" : 0,
  "Speed" : 9,
  "Resistances" : [],
- "Saves" : []
+ "SaveAdvantages" : []
   }</v>
       </c>
     </row>
@@ -61783,8 +61762,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L34" sqref="L34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -61842,7 +61821,7 @@
         <v>2873</v>
       </c>
       <c r="M1" s="146" t="s">
-        <v>2877</v>
+        <v>2924</v>
       </c>
       <c r="N1" s="188" t="s">
         <v>2801</v>
@@ -61901,7 +61880,7 @@
  ""Charisma"" : "&amp;J2&amp;",
  ""Speed"" : "&amp;SUBSTITUTE(K2,",",".")&amp;",
  ""Resistances"" : ["&amp;SUBSTITUTE(L2,",",".")&amp;"],
- ""Saves"" : ["&amp;SUBSTITUTE(L2,",",".")&amp;"],
+ ""SaveAdvantages"" : ["&amp;SUBSTITUTE(L2,",",".")&amp;"],
  ""ArmorCategories"" : ["&amp;'Sous-races'!N2&amp;"]
   }"</f>
         <v>"HIGH_ELF": {
@@ -61917,7 +61896,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : [],
- "Saves" : [],
+ "SaveAdvantages" : [],
  "ArmorCategories" : []
   }</v>
       </c>
@@ -61974,7 +61953,7 @@
  ""Charisma"" : "&amp;J3&amp;",
  ""Speed"" : "&amp;SUBSTITUTE(K3,",",".")&amp;",
  ""Resistances"" : ["&amp;SUBSTITUTE(L3,",",".")&amp;"],
- ""Saves"" : ["&amp;SUBSTITUTE(L3,",",".")&amp;"],
+ ""SaveAdvantages"" : ["&amp;SUBSTITUTE(L3,",",".")&amp;"],
  ""ArmorCategories"" : ["&amp;'Sous-races'!N3&amp;"]
   }"</f>
         <v>"WOODEN_ELF": {
@@ -61990,7 +61969,7 @@
  "Charisma" : 0,
  "Speed" : 10.5,
  "Resistances" : [],
- "Saves" : [],
+ "SaveAdvantages" : [],
  "ArmorCategories" : []
   }</v>
       </c>
@@ -62047,7 +62026,7 @@
  ""Charisma"" : "&amp;J4&amp;",
  ""Speed"" : "&amp;SUBSTITUTE(K4,",",".")&amp;",
  ""Resistances"" : ["&amp;SUBSTITUTE(L4,",",".")&amp;"],
- ""Saves"" : ["&amp;SUBSTITUTE(L4,",",".")&amp;"],
+ ""SaveAdvantages"" : ["&amp;SUBSTITUTE(L4,",",".")&amp;"],
  ""ArmorCategories"" : ["&amp;'Sous-races'!N4&amp;"]
   }"</f>
         <v>"DROW": {
@@ -62063,7 +62042,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : [],
- "Saves" : [],
+ "SaveAdvantages" : [],
  "ArmorCategories" : []
   }</v>
       </c>
@@ -62120,7 +62099,7 @@
  ""Charisma"" : "&amp;J5&amp;",
  ""Speed"" : "&amp;SUBSTITUTE(K5,",",".")&amp;",
  ""Resistances"" : ["&amp;SUBSTITUTE(L5,",",".")&amp;"],
- ""Saves"" : ["&amp;SUBSTITUTE(L5,",",".")&amp;"],
+ ""SaveAdvantages"" : ["&amp;SUBSTITUTE(L5,",",".")&amp;"],
  ""ArmorCategories"" : ["&amp;'Sous-races'!N5&amp;"]
   }"</f>
         <v>"LIGHT_FOOT_HALFELIN": {
@@ -62136,7 +62115,7 @@
  "Charisma" : 1,
  "Speed" : 0,
  "Resistances" : [],
- "Saves" : [],
+ "SaveAdvantages" : [],
  "ArmorCategories" : []
   }</v>
       </c>
@@ -62197,7 +62176,7 @@
  ""Charisma"" : "&amp;J6&amp;",
  ""Speed"" : "&amp;SUBSTITUTE(K6,",",".")&amp;",
  ""Resistances"" : ["&amp;SUBSTITUTE(L6,",",".")&amp;"],
- ""Saves"" : ["&amp;SUBSTITUTE(L6,",",".")&amp;"],
+ ""SaveAdvantages"" : ["&amp;SUBSTITUTE(L6,",",".")&amp;"],
  ""ArmorCategories"" : ["&amp;'Sous-races'!N6&amp;"]
   }"</f>
         <v>"ROBUST_HALFELIN": {
@@ -62213,7 +62192,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : ["Poisonned"],
- "Saves" : ["Poisonned"],
+ "SaveAdvantages" : ["Poisonned"],
  "ArmorCategories" : []
   }</v>
       </c>
@@ -62270,7 +62249,7 @@
  ""Charisma"" : "&amp;J7&amp;",
  ""Speed"" : "&amp;SUBSTITUTE(K7,",",".")&amp;",
  ""Resistances"" : ["&amp;SUBSTITUTE(L7,",",".")&amp;"],
- ""Saves"" : ["&amp;SUBSTITUTE(L7,",",".")&amp;"],
+ ""SaveAdvantages"" : ["&amp;SUBSTITUTE(L7,",",".")&amp;"],
  ""ArmorCategories"" : ["&amp;'Sous-races'!N7&amp;"]
   }"</f>
         <v>"HILLS_DWARF": {
@@ -62286,7 +62265,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : [],
- "Saves" : [],
+ "SaveAdvantages" : [],
  "ArmorCategories" : []
   }</v>
       </c>
@@ -62345,7 +62324,7 @@
  ""Charisma"" : "&amp;J8&amp;",
  ""Speed"" : "&amp;SUBSTITUTE(K8,",",".")&amp;",
  ""Resistances"" : ["&amp;SUBSTITUTE(L8,",",".")&amp;"],
- ""Saves"" : ["&amp;SUBSTITUTE(L8,",",".")&amp;"],
+ ""SaveAdvantages"" : ["&amp;SUBSTITUTE(L8,",",".")&amp;"],
  ""ArmorCategories"" : ["&amp;'Sous-races'!N8&amp;"]
   }"</f>
         <v>"MONTAINS_DWARF": {
@@ -62361,7 +62340,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : [],
- "Saves" : [],
+ "SaveAdvantages" : [],
  "ArmorCategories" : ["1_LIGHT", "2_MID"]
   }</v>
       </c>
@@ -62418,7 +62397,7 @@
  ""Charisma"" : "&amp;J9&amp;",
  ""Speed"" : "&amp;SUBSTITUTE(K9,",",".")&amp;",
  ""Resistances"" : ["&amp;SUBSTITUTE(L9,",",".")&amp;"],
- ""Saves"" : ["&amp;SUBSTITUTE(L9,",",".")&amp;"],
+ ""SaveAdvantages"" : ["&amp;SUBSTITUTE(L9,",",".")&amp;"],
  ""ArmorCategories"" : ["&amp;'Sous-races'!N9&amp;"]
   }"</f>
         <v>"FORESTS_GNOME": {
@@ -62434,7 +62413,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : [],
- "Saves" : [],
+ "SaveAdvantages" : [],
  "ArmorCategories" : []
   }</v>
       </c>
@@ -62491,7 +62470,7 @@
  ""Charisma"" : "&amp;J10&amp;",
  ""Speed"" : "&amp;SUBSTITUTE(K10,",",".")&amp;",
  ""Resistances"" : ["&amp;SUBSTITUTE(L10,",",".")&amp;"],
- ""Saves"" : ["&amp;SUBSTITUTE(L10,",",".")&amp;"],
+ ""SaveAdvantages"" : ["&amp;SUBSTITUTE(L10,",",".")&amp;"],
  ""ArmorCategories"" : ["&amp;'Sous-races'!N10&amp;"]
   }"</f>
         <v>"ROCKS_GNOME": {
@@ -62507,7 +62486,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : [],
- "Saves" : [],
+ "SaveAdvantages" : [],
  "ArmorCategories" : []
   }</v>
       </c>
@@ -62564,7 +62543,7 @@
  ""Charisma"" : "&amp;J11&amp;",
  ""Speed"" : "&amp;SUBSTITUTE(K11,",",".")&amp;",
  ""Resistances"" : ["&amp;SUBSTITUTE(L11,",",".")&amp;"],
- ""Saves"" : ["&amp;SUBSTITUTE(L11,",",".")&amp;"],
+ ""SaveAdvantages"" : ["&amp;SUBSTITUTE(L11,",",".")&amp;"],
  ""ArmorCategories"" : ["&amp;'Sous-races'!N11&amp;"]
   }"</f>
         <v>"DEPTH_GNOME": {
@@ -62580,7 +62559,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : [],
- "Saves" : [],
+ "SaveAdvantages" : [],
  "ArmorCategories" : []
   }</v>
       </c>
@@ -62637,7 +62616,7 @@
  ""Charisma"" : "&amp;J12&amp;",
  ""Speed"" : "&amp;SUBSTITUTE(K12,",",".")&amp;",
  ""Resistances"" : ["&amp;SUBSTITUTE(L12,",",".")&amp;"],
- ""Saves"" : ["&amp;SUBSTITUTE(L12,",",".")&amp;"],
+ ""SaveAdvantages"" : ["&amp;SUBSTITUTE(L12,",",".")&amp;"],
  ""ArmorCategories"" : ["&amp;'Sous-races'!N12&amp;"]
   }"</f>
         <v>"AIR_GENASI": {
@@ -62653,7 +62632,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : [],
- "Saves" : [],
+ "SaveAdvantages" : [],
  "ArmorCategories" : []
   }</v>
       </c>
@@ -62710,7 +62689,7 @@
  ""Charisma"" : "&amp;J13&amp;",
  ""Speed"" : "&amp;SUBSTITUTE(K13,",",".")&amp;",
  ""Resistances"" : ["&amp;SUBSTITUTE(L13,",",".")&amp;"],
- ""Saves"" : ["&amp;SUBSTITUTE(L13,",",".")&amp;"],
+ ""SaveAdvantages"" : ["&amp;SUBSTITUTE(L13,",",".")&amp;"],
  ""ArmorCategories"" : ["&amp;'Sous-races'!N13&amp;"]
   }"</f>
         <v>"EARTH_GENASI": {
@@ -62726,7 +62705,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : [],
- "Saves" : [],
+ "SaveAdvantages" : [],
  "ArmorCategories" : []
   }</v>
       </c>
@@ -62785,7 +62764,7 @@
  ""Charisma"" : "&amp;J14&amp;",
  ""Speed"" : "&amp;SUBSTITUTE(K14,",",".")&amp;",
  ""Resistances"" : ["&amp;SUBSTITUTE(L14,",",".")&amp;"],
- ""Saves"" : ["&amp;SUBSTITUTE(L14,",",".")&amp;"],
+ ""SaveAdvantages"" : ["&amp;SUBSTITUTE(L14,",",".")&amp;"],
  ""ArmorCategories"" : ["&amp;'Sous-races'!N14&amp;"]
   }"</f>
         <v>"FIRE_GENASI": {
@@ -62801,7 +62780,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : ["Burned"],
- "Saves" : ["Burned"],
+ "SaveAdvantages" : ["Burned"],
  "ArmorCategories" : []
   }</v>
       </c>
@@ -62860,7 +62839,7 @@
  ""Charisma"" : "&amp;J15&amp;",
  ""Speed"" : "&amp;SUBSTITUTE(K15,",",".")&amp;",
  ""Resistances"" : ["&amp;SUBSTITUTE(L15,",",".")&amp;"],
- ""Saves"" : ["&amp;SUBSTITUTE(L15,",",".")&amp;"],
+ ""SaveAdvantages"" : ["&amp;SUBSTITUTE(L15,",",".")&amp;"],
  ""ArmorCategories"" : ["&amp;'Sous-races'!N15&amp;"]
   }"</f>
         <v>"WATER_GENASI": {
@@ -62876,7 +62855,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : ["Acidified"],
- "Saves" : ["Acidified"],
+ "SaveAdvantages" : ["Acidified"],
  "ArmorCategories" : []
   }</v>
       </c>
@@ -62932,7 +62911,7 @@
  ""Charisma"" : "&amp;J16&amp;",
  ""Speed"" : "&amp;SUBSTITUTE(K16,",",".")&amp;",
  ""Resistances"" : ["&amp;SUBSTITUTE(L16,",",".")&amp;"],
- ""Saves"" : ["&amp;SUBSTITUTE(L16,",",".")&amp;"],
+ ""SaveAdvantages"" : ["&amp;SUBSTITUTE(L16,",",".")&amp;"],
  ""ArmorCategories"" : ["&amp;'Sous-races'!N16&amp;"]
   }"</f>
         <v>"HUMAN": {
@@ -62948,7 +62927,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : [],
- "Saves" : [],
+ "SaveAdvantages" : [],
  "ArmorCategories" : []
   }</v>
       </c>
@@ -63004,7 +62983,7 @@
  ""Charisma"" : "&amp;J17&amp;",
  ""Speed"" : "&amp;SUBSTITUTE(K17,",",".")&amp;",
  ""Resistances"" : ["&amp;SUBSTITUTE(L17,",",".")&amp;"],
- ""Saves"" : ["&amp;SUBSTITUTE(L17,",",".")&amp;"],
+ ""SaveAdvantages"" : ["&amp;SUBSTITUTE(L17,",",".")&amp;"],
  ""ArmorCategories"" : ["&amp;'Sous-races'!N17&amp;"]
   }"</f>
         <v>"HALF_ELF": {
@@ -63020,7 +62999,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : [],
- "Saves" : [],
+ "SaveAdvantages" : [],
  "ArmorCategories" : []
   }</v>
       </c>
@@ -63076,7 +63055,7 @@
  ""Charisma"" : "&amp;J18&amp;",
  ""Speed"" : "&amp;SUBSTITUTE(K18,",",".")&amp;",
  ""Resistances"" : ["&amp;SUBSTITUTE(L18,",",".")&amp;"],
- ""Saves"" : ["&amp;SUBSTITUTE(L18,",",".")&amp;"],
+ ""SaveAdvantages"" : ["&amp;SUBSTITUTE(L18,",",".")&amp;"],
  ""ArmorCategories"" : ["&amp;'Sous-races'!N18&amp;"]
   }"</f>
         <v>"HALF_ORC": {
@@ -63092,7 +63071,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : [],
- "Saves" : [],
+ "SaveAdvantages" : [],
  "ArmorCategories" : []
   }</v>
       </c>
@@ -63150,7 +63129,7 @@
  ""Charisma"" : "&amp;J19&amp;",
  ""Speed"" : "&amp;SUBSTITUTE(K19,",",".")&amp;",
  ""Resistances"" : ["&amp;SUBSTITUTE(L19,",",".")&amp;"],
- ""Saves"" : ["&amp;SUBSTITUTE(L19,",",".")&amp;"],
+ ""SaveAdvantages"" : ["&amp;SUBSTITUTE(L19,",",".")&amp;"],
  ""ArmorCategories"" : ["&amp;'Sous-races'!N19&amp;"]
   }"</f>
         <v>"WHITE_DRAGON": {
@@ -63166,7 +63145,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : ["Cold"],
- "Saves" : ["Cold"],
+ "SaveAdvantages" : ["Cold"],
  "ArmorCategories" : []
   }</v>
       </c>
@@ -63224,7 +63203,7 @@
  ""Charisma"" : "&amp;J20&amp;",
  ""Speed"" : "&amp;SUBSTITUTE(K20,",",".")&amp;",
  ""Resistances"" : ["&amp;SUBSTITUTE(L20,",",".")&amp;"],
- ""Saves"" : ["&amp;SUBSTITUTE(L20,",",".")&amp;"],
+ ""SaveAdvantages"" : ["&amp;SUBSTITUTE(L20,",",".")&amp;"],
  ""ArmorCategories"" : ["&amp;'Sous-races'!N20&amp;"]
   }"</f>
         <v>"BLUE_DRAGON": {
@@ -63240,7 +63219,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : ["Electrified"],
- "Saves" : ["Electrified"],
+ "SaveAdvantages" : ["Electrified"],
  "ArmorCategories" : []
   }</v>
       </c>
@@ -63298,7 +63277,7 @@
  ""Charisma"" : "&amp;J21&amp;",
  ""Speed"" : "&amp;SUBSTITUTE(K21,",",".")&amp;",
  ""Resistances"" : ["&amp;SUBSTITUTE(L21,",",".")&amp;"],
- ""Saves"" : ["&amp;SUBSTITUTE(L21,",",".")&amp;"],
+ ""SaveAdvantages"" : ["&amp;SUBSTITUTE(L21,",",".")&amp;"],
  ""ArmorCategories"" : ["&amp;'Sous-races'!N21&amp;"]
   }"</f>
         <v>"BLACK_DRAGON": {
@@ -63314,7 +63293,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : ["Acidified"],
- "Saves" : ["Acidified"],
+ "SaveAdvantages" : ["Acidified"],
  "ArmorCategories" : []
   }</v>
       </c>
@@ -63372,7 +63351,7 @@
  ""Charisma"" : "&amp;J22&amp;",
  ""Speed"" : "&amp;SUBSTITUTE(K22,",",".")&amp;",
  ""Resistances"" : ["&amp;SUBSTITUTE(L22,",",".")&amp;"],
- ""Saves"" : ["&amp;SUBSTITUTE(L22,",",".")&amp;"],
+ ""SaveAdvantages"" : ["&amp;SUBSTITUTE(L22,",",".")&amp;"],
  ""ArmorCategories"" : ["&amp;'Sous-races'!N22&amp;"]
   }"</f>
         <v>"RED_DRAGON": {
@@ -63388,7 +63367,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : ["Burned"],
- "Saves" : ["Burned"],
+ "SaveAdvantages" : ["Burned"],
  "ArmorCategories" : []
   }</v>
       </c>
@@ -63446,7 +63425,7 @@
  ""Charisma"" : "&amp;J23&amp;",
  ""Speed"" : "&amp;SUBSTITUTE(K23,",",".")&amp;",
  ""Resistances"" : ["&amp;SUBSTITUTE(L23,",",".")&amp;"],
- ""Saves"" : ["&amp;SUBSTITUTE(L23,",",".")&amp;"],
+ ""SaveAdvantages"" : ["&amp;SUBSTITUTE(L23,",",".")&amp;"],
  ""ArmorCategories"" : ["&amp;'Sous-races'!N23&amp;"]
   }"</f>
         <v>"GREEN_DRAGON": {
@@ -63462,7 +63441,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : ["Poisonned"],
- "Saves" : ["Poisonned"],
+ "SaveAdvantages" : ["Poisonned"],
  "ArmorCategories" : []
   }</v>
       </c>
@@ -63520,7 +63499,7 @@
  ""Charisma"" : "&amp;J24&amp;",
  ""Speed"" : "&amp;SUBSTITUTE(K24,",",".")&amp;",
  ""Resistances"" : ["&amp;SUBSTITUTE(L24,",",".")&amp;"],
- ""Saves"" : ["&amp;SUBSTITUTE(L24,",",".")&amp;"],
+ ""SaveAdvantages"" : ["&amp;SUBSTITUTE(L24,",",".")&amp;"],
  ""ArmorCategories"" : ["&amp;'Sous-races'!N24&amp;"]
   }"</f>
         <v>"BRASS_DRAGON": {
@@ -63536,7 +63515,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : ["Burned"],
- "Saves" : ["Burned"],
+ "SaveAdvantages" : ["Burned"],
  "ArmorCategories" : []
   }</v>
       </c>
@@ -63594,7 +63573,7 @@
  ""Charisma"" : "&amp;J25&amp;",
  ""Speed"" : "&amp;SUBSTITUTE(K25,",",".")&amp;",
  ""Resistances"" : ["&amp;SUBSTITUTE(L25,",",".")&amp;"],
- ""Saves"" : ["&amp;SUBSTITUTE(L25,",",".")&amp;"],
+ ""SaveAdvantages"" : ["&amp;SUBSTITUTE(L25,",",".")&amp;"],
  ""ArmorCategories"" : ["&amp;'Sous-races'!N25&amp;"]
   }"</f>
         <v>"SILVER_DRAGON": {
@@ -63610,7 +63589,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : ["Cold"],
- "Saves" : ["Cold"],
+ "SaveAdvantages" : ["Cold"],
  "ArmorCategories" : []
   }</v>
       </c>
@@ -63668,7 +63647,7 @@
  ""Charisma"" : "&amp;J26&amp;",
  ""Speed"" : "&amp;SUBSTITUTE(K26,",",".")&amp;",
  ""Resistances"" : ["&amp;SUBSTITUTE(L26,",",".")&amp;"],
- ""Saves"" : ["&amp;SUBSTITUTE(L26,",",".")&amp;"],
+ ""SaveAdvantages"" : ["&amp;SUBSTITUTE(L26,",",".")&amp;"],
  ""ArmorCategories"" : ["&amp;'Sous-races'!N26&amp;"]
   }"</f>
         <v>"BRONZE_DRAGON": {
@@ -63684,7 +63663,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : ["Electrified"],
- "Saves" : ["Electrified"],
+ "SaveAdvantages" : ["Electrified"],
  "ArmorCategories" : []
   }</v>
       </c>
@@ -63742,7 +63721,7 @@
  ""Charisma"" : "&amp;J27&amp;",
  ""Speed"" : "&amp;SUBSTITUTE(K27,",",".")&amp;",
  ""Resistances"" : ["&amp;SUBSTITUTE(L27,",",".")&amp;"],
- ""Saves"" : ["&amp;SUBSTITUTE(L27,",",".")&amp;"],
+ ""SaveAdvantages"" : ["&amp;SUBSTITUTE(L27,",",".")&amp;"],
  ""ArmorCategories"" : ["&amp;'Sous-races'!N27&amp;"]
   }"</f>
         <v>"COPPER_DRAGON": {
@@ -63758,7 +63737,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : ["Acidified"],
- "Saves" : ["Acidified"],
+ "SaveAdvantages" : ["Acidified"],
  "ArmorCategories" : []
   }</v>
       </c>
@@ -63816,7 +63795,7 @@
  ""Charisma"" : "&amp;J28&amp;",
  ""Speed"" : "&amp;SUBSTITUTE(K28,",",".")&amp;",
  ""Resistances"" : ["&amp;SUBSTITUTE(L28,",",".")&amp;"],
- ""Saves"" : ["&amp;SUBSTITUTE(L28,",",".")&amp;"],
+ ""SaveAdvantages"" : ["&amp;SUBSTITUTE(L28,",",".")&amp;"],
  ""ArmorCategories"" : ["&amp;'Sous-races'!N28&amp;"]
   }"</f>
         <v>"GOLD_DRAGON": {
@@ -63832,7 +63811,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : ["Burned"],
- "Saves" : ["Burned"],
+ "SaveAdvantages" : ["Burned"],
  "ArmorCategories" : []
   }</v>
       </c>
@@ -63890,7 +63869,7 @@
  ""Charisma"" : "&amp;J29&amp;",
  ""Speed"" : "&amp;SUBSTITUTE(K29,",",".")&amp;",
  ""Resistances"" : ["&amp;SUBSTITUTE(L29,",",".")&amp;"],
- ""Saves"" : ["&amp;SUBSTITUTE(L29,",",".")&amp;"],
+ ""SaveAdvantages"" : ["&amp;SUBSTITUTE(L29,",",".")&amp;"],
  ""ArmorCategories"" : ["&amp;'Sous-races'!N29&amp;"]
   }"</f>
         <v>"TIEFFLING": {
@@ -63906,7 +63885,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : ["Burned"],
- "Saves" : ["Burned"],
+ "SaveAdvantages" : ["Burned"],
  "ArmorCategories" : []
   }</v>
       </c>
@@ -63962,7 +63941,7 @@
  ""Charisma"" : "&amp;J30&amp;",
  ""Speed"" : "&amp;SUBSTITUTE(K30,",",".")&amp;",
  ""Resistances"" : ["&amp;SUBSTITUTE(L30,",",".")&amp;"],
- ""Saves"" : ["&amp;SUBSTITUTE(L30,",",".")&amp;"],
+ ""SaveAdvantages"" : ["&amp;SUBSTITUTE(L30,",",".")&amp;"],
  ""ArmorCategories"" : ["&amp;'Sous-races'!N30&amp;"]
   }"</f>
         <v>"AARAKOCRA": {
@@ -63978,7 +63957,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : [],
- "Saves" : [],
+ "SaveAdvantages" : [],
  "ArmorCategories" : []
   }</v>
       </c>
@@ -64034,7 +64013,7 @@
  ""Charisma"" : "&amp;J31&amp;",
  ""Speed"" : "&amp;SUBSTITUTE(K31,",",".")&amp;",
  ""Resistances"" : ["&amp;SUBSTITUTE(L31,",",".")&amp;"],
- ""Saves"" : ["&amp;SUBSTITUTE(L31,",",".")&amp;"],
+ ""SaveAdvantages"" : ["&amp;SUBSTITUTE(L31,",",".")&amp;"],
  ""ArmorCategories"" : ["&amp;'Sous-races'!N31&amp;"]
   }"</f>
         <v>"GOLIATH": {
@@ -64050,7 +64029,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : [],
- "Saves" : [],
+ "SaveAdvantages" : [],
  "ArmorCategories" : []
   }</v>
       </c>
@@ -64104,7 +64083,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : [],
- "Saves" : [],
+ "SaveAdvantages" : [],
  "ArmorCategories" : []
   },
 "WOODEN_ELF": {
@@ -64120,7 +64099,7 @@
  "Charisma" : 0,
  "Speed" : 10.5,
  "Resistances" : [],
- "Saves" : [],
+ "SaveAdvantages" : [],
  "ArmorCategories" : []
   },
 "DROW": {
@@ -64136,7 +64115,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : [],
- "Saves" : [],
+ "SaveAdvantages" : [],
  "ArmorCategories" : []
   },
 "LIGHT_FOOT_HALFELIN": {
@@ -64152,7 +64131,7 @@
  "Charisma" : 1,
  "Speed" : 0,
  "Resistances" : [],
- "Saves" : [],
+ "SaveAdvantages" : [],
  "ArmorCategories" : []
   },
 "ROBUST_HALFELIN": {
@@ -64168,7 +64147,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : ["Poisonned"],
- "Saves" : ["Poisonned"],
+ "SaveAdvantages" : ["Poisonned"],
  "ArmorCategories" : []
   },
 "HILLS_DWARF": {
@@ -64184,7 +64163,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : [],
- "Saves" : [],
+ "SaveAdvantages" : [],
  "ArmorCategories" : []
   },
 "MONTAINS_DWARF": {
@@ -64200,7 +64179,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : [],
- "Saves" : [],
+ "SaveAdvantages" : [],
  "ArmorCategories" : ["1_LIGHT", "2_MID"]
   },
 "FORESTS_GNOME": {
@@ -64216,7 +64195,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : [],
- "Saves" : [],
+ "SaveAdvantages" : [],
  "ArmorCategories" : []
   },
 "ROCKS_GNOME": {
@@ -64232,7 +64211,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : [],
- "Saves" : [],
+ "SaveAdvantages" : [],
  "ArmorCategories" : []
   },
 "DEPTH_GNOME": {
@@ -64248,7 +64227,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : [],
- "Saves" : [],
+ "SaveAdvantages" : [],
  "ArmorCategories" : []
   },
 "AIR_GENASI": {
@@ -64264,7 +64243,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : [],
- "Saves" : [],
+ "SaveAdvantages" : [],
  "ArmorCategories" : []
   },
 "EARTH_GENASI": {
@@ -64280,7 +64259,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : [],
- "Saves" : [],
+ "SaveAdvantages" : [],
  "ArmorCategories" : []
   },
 "FIRE_GENASI": {
@@ -64296,7 +64275,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : ["Burned"],
- "Saves" : ["Burned"],
+ "SaveAdvantages" : ["Burned"],
  "ArmorCategories" : []
   },
 "WATER_GENASI": {
@@ -64312,7 +64291,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : ["Acidified"],
- "Saves" : ["Acidified"],
+ "SaveAdvantages" : ["Acidified"],
  "ArmorCategories" : []
   },
 "HUMAN": {
@@ -64328,7 +64307,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : [],
- "Saves" : [],
+ "SaveAdvantages" : [],
  "ArmorCategories" : []
   },
 "HALF_ELF": {
@@ -64344,7 +64323,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : [],
- "Saves" : [],
+ "SaveAdvantages" : [],
  "ArmorCategories" : []
   },
 "HALF_ORC": {
@@ -64360,7 +64339,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : [],
- "Saves" : [],
+ "SaveAdvantages" : [],
  "ArmorCategories" : []
   },
 "WHITE_DRAGON": {
@@ -64376,7 +64355,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : ["Cold"],
- "Saves" : ["Cold"],
+ "SaveAdvantages" : ["Cold"],
  "ArmorCategories" : []
   },
 "BLUE_DRAGON": {
@@ -64392,7 +64371,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : ["Electrified"],
- "Saves" : ["Electrified"],
+ "SaveAdvantages" : ["Electrified"],
  "ArmorCategories" : []
   },
 "BLACK_DRAGON": {
@@ -64408,7 +64387,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : ["Acidified"],
- "Saves" : ["Acidified"],
+ "SaveAdvantages" : ["Acidified"],
  "ArmorCategories" : []
   },
 "RED_DRAGON": {
@@ -64424,7 +64403,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : ["Burned"],
- "Saves" : ["Burned"],
+ "SaveAdvantages" : ["Burned"],
  "ArmorCategories" : []
   },
 "GREEN_DRAGON": {
@@ -64440,7 +64419,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : ["Poisonned"],
- "Saves" : ["Poisonned"],
+ "SaveAdvantages" : ["Poisonned"],
  "ArmorCategories" : []
   },
 "BRASS_DRAGON": {
@@ -64456,7 +64435,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : ["Burned"],
- "Saves" : ["Burned"],
+ "SaveAdvantages" : ["Burned"],
  "ArmorCategories" : []
   },
 "SILVER_DRAGON": {
@@ -64472,7 +64451,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : ["Cold"],
- "Saves" : ["Cold"],
+ "SaveAdvantages" : ["Cold"],
  "ArmorCategories" : []
   },
 "BRONZE_DRAGON": {
@@ -64488,7 +64467,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : ["Electrified"],
- "Saves" : ["Electrified"],
+ "SaveAdvantages" : ["Electrified"],
  "ArmorCategories" : []
   },
 "COPPER_DRAGON": {
@@ -64504,7 +64483,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : ["Acidified"],
- "Saves" : ["Acidified"],
+ "SaveAdvantages" : ["Acidified"],
  "ArmorCategories" : []
   },
 "GOLD_DRAGON": {
@@ -64520,7 +64499,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : ["Burned"],
- "Saves" : ["Burned"],
+ "SaveAdvantages" : ["Burned"],
  "ArmorCategories" : []
   },
 "TIEFFLING": {
@@ -64536,7 +64515,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : ["Burned"],
- "Saves" : ["Burned"],
+ "SaveAdvantages" : ["Burned"],
  "ArmorCategories" : []
   },
 "AARAKOCRA": {
@@ -64552,7 +64531,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : [],
- "Saves" : [],
+ "SaveAdvantages" : [],
  "ArmorCategories" : []
   },
 "GOLIATH": {
@@ -64568,7 +64547,7 @@
  "Charisma" : 0,
  "Speed" : 0,
  "Resistances" : [],
- "Saves" : [],
+ "SaveAdvantages" : [],
  "ArmorCategories" : []
   }</v>
       </c>
@@ -64610,11 +64589,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="O1" sqref="O1"/>
       <selection pane="bottomLeft" activeCell="A23" sqref="A23"/>
-      <selection pane="bottomRight" activeCell="Q11" sqref="Q11"/>
+      <selection pane="bottomRight" activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -64629,7 +64608,8 @@
     <col min="12" max="12" width="17.42578125" customWidth="1"/>
     <col min="13" max="13" width="35.140625" customWidth="1"/>
     <col min="14" max="14" width="53" customWidth="1"/>
-    <col min="15" max="16" width="41.7109375" customWidth="1"/>
+    <col min="15" max="15" width="41.7109375" customWidth="1"/>
+    <col min="16" max="16" width="18.5703125" customWidth="1"/>
     <col min="17" max="17" width="8.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -64676,10 +64656,10 @@
       <c r="N1" s="146" t="s">
         <v>2798</v>
       </c>
-      <c r="O1" s="188" t="s">
+      <c r="O1" s="146" t="s">
         <v>2801</v>
       </c>
-      <c r="P1" s="146" t="s">
+      <c r="P1" s="188" t="s">
         <v>2877</v>
       </c>
       <c r="Q1" s="100"/>
@@ -65344,7 +65324,7 @@
         <v>2805</v>
       </c>
       <c r="N11" s="187"/>
-      <c r="O11" s="239" t="s">
+      <c r="O11" s="226" t="s">
         <v>2912</v>
       </c>
       <c r="P11" s="198" t="s">
@@ -65478,7 +65458,7 @@
         <v>2799</v>
       </c>
       <c r="N13" s="189"/>
-      <c r="O13" s="240" t="s">
+      <c r="O13" s="227" t="s">
         <v>2911</v>
       </c>
       <c r="P13" s="199" t="s">
@@ -65773,58 +65753,58 @@
   <sheetData>
     <row r="1" spans="1:112">
       <c r="A1" s="176"/>
-      <c r="B1" s="227" t="s">
+      <c r="B1" s="230" t="s">
         <v>385</v>
       </c>
-      <c r="C1" s="227"/>
-      <c r="D1" s="227"/>
-      <c r="E1" s="227"/>
-      <c r="F1" s="228"/>
-      <c r="G1" s="226" t="s">
+      <c r="C1" s="230"/>
+      <c r="D1" s="230"/>
+      <c r="E1" s="230"/>
+      <c r="F1" s="232"/>
+      <c r="G1" s="231" t="s">
         <v>386</v>
       </c>
-      <c r="H1" s="227"/>
-      <c r="I1" s="227"/>
-      <c r="J1" s="227"/>
-      <c r="K1" s="227"/>
-      <c r="L1" s="227"/>
-      <c r="M1" s="227"/>
-      <c r="N1" s="227"/>
-      <c r="O1" s="227"/>
-      <c r="P1" s="227"/>
-      <c r="Q1" s="227"/>
-      <c r="R1" s="227"/>
-      <c r="S1" s="227"/>
+      <c r="H1" s="230"/>
+      <c r="I1" s="230"/>
+      <c r="J1" s="230"/>
+      <c r="K1" s="230"/>
+      <c r="L1" s="230"/>
+      <c r="M1" s="230"/>
+      <c r="N1" s="230"/>
+      <c r="O1" s="230"/>
+      <c r="P1" s="230"/>
+      <c r="Q1" s="230"/>
+      <c r="R1" s="230"/>
+      <c r="S1" s="230"/>
       <c r="T1" s="164"/>
-      <c r="U1" s="227" t="s">
+      <c r="U1" s="230" t="s">
         <v>387</v>
       </c>
-      <c r="V1" s="227"/>
-      <c r="W1" s="227"/>
-      <c r="X1" s="227"/>
-      <c r="Y1" s="227"/>
-      <c r="Z1" s="227"/>
-      <c r="AA1" s="227"/>
-      <c r="AB1" s="227"/>
-      <c r="AC1" s="227"/>
-      <c r="AD1" s="227"/>
-      <c r="AE1" s="227"/>
-      <c r="AF1" s="227"/>
+      <c r="V1" s="230"/>
+      <c r="W1" s="230"/>
+      <c r="X1" s="230"/>
+      <c r="Y1" s="230"/>
+      <c r="Z1" s="230"/>
+      <c r="AA1" s="230"/>
+      <c r="AB1" s="230"/>
+      <c r="AC1" s="230"/>
+      <c r="AD1" s="230"/>
+      <c r="AE1" s="230"/>
+      <c r="AF1" s="230"/>
       <c r="AG1" s="150"/>
-      <c r="AH1" s="226" t="s">
+      <c r="AH1" s="231" t="s">
         <v>388</v>
       </c>
-      <c r="AI1" s="227"/>
-      <c r="AJ1" s="227"/>
-      <c r="AK1" s="227"/>
-      <c r="AL1" s="227"/>
-      <c r="AM1" s="227"/>
-      <c r="AN1" s="227"/>
-      <c r="AO1" s="227"/>
-      <c r="AP1" s="227"/>
-      <c r="AQ1" s="227"/>
-      <c r="AR1" s="227"/>
-      <c r="AS1" s="228"/>
+      <c r="AI1" s="230"/>
+      <c r="AJ1" s="230"/>
+      <c r="AK1" s="230"/>
+      <c r="AL1" s="230"/>
+      <c r="AM1" s="230"/>
+      <c r="AN1" s="230"/>
+      <c r="AO1" s="230"/>
+      <c r="AP1" s="230"/>
+      <c r="AQ1" s="230"/>
+      <c r="AR1" s="230"/>
+      <c r="AS1" s="232"/>
       <c r="AT1" s="150"/>
       <c r="AU1" s="229" t="s">
         <v>389</v>
@@ -65843,70 +65823,70 @@
       <c r="BG1" s="229"/>
       <c r="BH1" s="229"/>
       <c r="BI1" s="160"/>
-      <c r="BJ1" s="226" t="s">
+      <c r="BJ1" s="231" t="s">
         <v>390</v>
       </c>
-      <c r="BK1" s="227"/>
+      <c r="BK1" s="230"/>
       <c r="BL1" s="164"/>
-      <c r="BM1" s="227" t="s">
+      <c r="BM1" s="230" t="s">
         <v>391</v>
       </c>
-      <c r="BN1" s="227"/>
-      <c r="BO1" s="227"/>
-      <c r="BP1" s="227"/>
-      <c r="BQ1" s="227"/>
-      <c r="BR1" s="227"/>
-      <c r="BS1" s="227"/>
-      <c r="BT1" s="227"/>
-      <c r="BU1" s="227"/>
-      <c r="BV1" s="227"/>
-      <c r="BW1" s="227"/>
-      <c r="BX1" s="227"/>
+      <c r="BN1" s="230"/>
+      <c r="BO1" s="230"/>
+      <c r="BP1" s="230"/>
+      <c r="BQ1" s="230"/>
+      <c r="BR1" s="230"/>
+      <c r="BS1" s="230"/>
+      <c r="BT1" s="230"/>
+      <c r="BU1" s="230"/>
+      <c r="BV1" s="230"/>
+      <c r="BW1" s="230"/>
+      <c r="BX1" s="230"/>
       <c r="BY1" s="150"/>
-      <c r="BZ1" s="226" t="s">
+      <c r="BZ1" s="231" t="s">
         <v>393</v>
       </c>
-      <c r="CA1" s="227"/>
-      <c r="CB1" s="227"/>
-      <c r="CC1" s="227"/>
-      <c r="CD1" s="227"/>
+      <c r="CA1" s="230"/>
+      <c r="CB1" s="230"/>
+      <c r="CC1" s="230"/>
+      <c r="CD1" s="230"/>
       <c r="CE1" s="164"/>
-      <c r="CF1" s="226" t="s">
+      <c r="CF1" s="231" t="s">
         <v>12</v>
       </c>
-      <c r="CG1" s="227"/>
-      <c r="CH1" s="227"/>
-      <c r="CI1" s="227"/>
-      <c r="CJ1" s="227"/>
-      <c r="CK1" s="227"/>
-      <c r="CL1" s="227"/>
+      <c r="CG1" s="230"/>
+      <c r="CH1" s="230"/>
+      <c r="CI1" s="230"/>
+      <c r="CJ1" s="230"/>
+      <c r="CK1" s="230"/>
+      <c r="CL1" s="230"/>
       <c r="CM1" s="164"/>
-      <c r="CN1" s="227" t="s">
+      <c r="CN1" s="230" t="s">
         <v>394</v>
       </c>
-      <c r="CO1" s="227"/>
-      <c r="CP1" s="227"/>
-      <c r="CQ1" s="227"/>
-      <c r="CR1" s="227"/>
-      <c r="CS1" s="227"/>
-      <c r="CT1" s="227"/>
-      <c r="CU1" s="227"/>
+      <c r="CO1" s="230"/>
+      <c r="CP1" s="230"/>
+      <c r="CQ1" s="230"/>
+      <c r="CR1" s="230"/>
+      <c r="CS1" s="230"/>
+      <c r="CT1" s="230"/>
+      <c r="CU1" s="230"/>
       <c r="CV1" s="150"/>
-      <c r="CW1" s="230" t="s">
+      <c r="CW1" s="228" t="s">
         <v>395</v>
       </c>
       <c r="CX1" s="229"/>
       <c r="CY1" s="229"/>
       <c r="CZ1" s="174"/>
-      <c r="DA1" s="227" t="s">
+      <c r="DA1" s="230" t="s">
         <v>392</v>
       </c>
-      <c r="DB1" s="227"/>
-      <c r="DC1" s="227"/>
-      <c r="DD1" s="227"/>
-      <c r="DE1" s="227"/>
-      <c r="DF1" s="227"/>
-      <c r="DG1" s="227"/>
+      <c r="DB1" s="230"/>
+      <c r="DC1" s="230"/>
+      <c r="DD1" s="230"/>
+      <c r="DE1" s="230"/>
+      <c r="DF1" s="230"/>
+      <c r="DG1" s="230"/>
       <c r="DH1" s="185"/>
     </row>
     <row r="2" spans="1:112" s="122" customFormat="1" ht="15" customHeight="1">
@@ -80446,6 +80426,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="AH1:AS1"/>
+    <mergeCell ref="G1:S1"/>
+    <mergeCell ref="AU1:BH1"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="U1:AF1"/>
     <mergeCell ref="CW1:CY1"/>
     <mergeCell ref="DA1:DG1"/>
     <mergeCell ref="CF1:CL1"/>
@@ -80453,11 +80438,6 @@
     <mergeCell ref="BJ1:BK1"/>
     <mergeCell ref="BM1:BX1"/>
     <mergeCell ref="BZ1:CD1"/>
-    <mergeCell ref="AH1:AS1"/>
-    <mergeCell ref="G1:S1"/>
-    <mergeCell ref="AU1:BH1"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="U1:AF1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -80990,16 +80970,16 @@
       <c r="L1" s="108"/>
     </row>
     <row r="2" spans="1:13" ht="15" customHeight="1">
-      <c r="A2" s="231" t="s">
+      <c r="A2" s="233" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="232"/>
-      <c r="C2" s="232"/>
-      <c r="D2" s="232"/>
-      <c r="E2" s="232"/>
-      <c r="F2" s="232"/>
-      <c r="G2" s="232"/>
-      <c r="H2" s="233"/>
+      <c r="B2" s="234"/>
+      <c r="C2" s="234"/>
+      <c r="D2" s="234"/>
+      <c r="E2" s="234"/>
+      <c r="F2" s="234"/>
+      <c r="G2" s="234"/>
+      <c r="H2" s="235"/>
       <c r="I2" s="109"/>
       <c r="J2" s="109"/>
       <c r="K2" s="110"/>
@@ -81554,16 +81534,16 @@
       </c>
     </row>
     <row r="13" spans="1:13" ht="15" customHeight="1">
-      <c r="A13" s="234" t="s">
+      <c r="A13" s="236" t="s">
         <v>57</v>
       </c>
-      <c r="B13" s="235"/>
-      <c r="C13" s="235"/>
-      <c r="D13" s="235"/>
-      <c r="E13" s="235"/>
-      <c r="F13" s="235"/>
-      <c r="G13" s="235"/>
-      <c r="H13" s="236"/>
+      <c r="B13" s="237"/>
+      <c r="C13" s="237"/>
+      <c r="D13" s="237"/>
+      <c r="E13" s="237"/>
+      <c r="F13" s="237"/>
+      <c r="G13" s="237"/>
+      <c r="H13" s="238"/>
       <c r="I13" s="109"/>
       <c r="J13" s="109"/>
       <c r="K13" s="112"/>
@@ -81782,16 +81762,16 @@
       </c>
     </row>
     <row r="18" spans="1:13" ht="15" customHeight="1">
-      <c r="A18" s="234" t="s">
+      <c r="A18" s="236" t="s">
         <v>71</v>
       </c>
-      <c r="B18" s="235"/>
-      <c r="C18" s="235"/>
-      <c r="D18" s="235"/>
-      <c r="E18" s="235"/>
-      <c r="F18" s="235"/>
-      <c r="G18" s="235"/>
-      <c r="H18" s="236"/>
+      <c r="B18" s="237"/>
+      <c r="C18" s="237"/>
+      <c r="D18" s="237"/>
+      <c r="E18" s="237"/>
+      <c r="F18" s="237"/>
+      <c r="G18" s="237"/>
+      <c r="H18" s="238"/>
       <c r="I18" s="109"/>
       <c r="J18" s="109"/>
       <c r="K18" s="112"/>
@@ -82752,16 +82732,16 @@
       </c>
     </row>
     <row r="37" spans="1:13" ht="15" customHeight="1">
-      <c r="A37" s="234" t="s">
+      <c r="A37" s="236" t="s">
         <v>112</v>
       </c>
-      <c r="B37" s="235"/>
-      <c r="C37" s="235"/>
-      <c r="D37" s="235"/>
-      <c r="E37" s="235"/>
-      <c r="F37" s="235"/>
-      <c r="G37" s="235"/>
-      <c r="H37" s="236"/>
+      <c r="B37" s="237"/>
+      <c r="C37" s="237"/>
+      <c r="D37" s="237"/>
+      <c r="E37" s="237"/>
+      <c r="F37" s="237"/>
+      <c r="G37" s="237"/>
+      <c r="H37" s="238"/>
       <c r="I37" s="109"/>
       <c r="J37" s="109"/>
       <c r="K37" s="112"/>
@@ -83495,17 +83475,17 @@
       </c>
     </row>
     <row r="2" spans="1:14" s="126" customFormat="1" ht="15" customHeight="1">
-      <c r="A2" s="237" t="s">
+      <c r="A2" s="239" t="s">
         <v>488</v>
       </c>
-      <c r="B2" s="237"/>
-      <c r="C2" s="237"/>
-      <c r="D2" s="237"/>
-      <c r="E2" s="237"/>
-      <c r="F2" s="237"/>
-      <c r="G2" s="237"/>
-      <c r="H2" s="237"/>
-      <c r="I2" s="237"/>
+      <c r="B2" s="239"/>
+      <c r="C2" s="239"/>
+      <c r="D2" s="239"/>
+      <c r="E2" s="239"/>
+      <c r="F2" s="239"/>
+      <c r="G2" s="239"/>
+      <c r="H2" s="239"/>
+      <c r="I2" s="239"/>
     </row>
     <row r="3" spans="1:14" ht="15" customHeight="1">
       <c r="A3" s="116" t="s">
@@ -83692,17 +83672,17 @@
       </c>
     </row>
     <row r="6" spans="1:14" s="126" customFormat="1" ht="15" customHeight="1">
-      <c r="A6" s="237" t="s">
+      <c r="A6" s="239" t="s">
         <v>499</v>
       </c>
-      <c r="B6" s="237"/>
-      <c r="C6" s="237"/>
-      <c r="D6" s="237"/>
-      <c r="E6" s="237"/>
-      <c r="F6" s="237"/>
-      <c r="G6" s="237"/>
-      <c r="H6" s="237"/>
-      <c r="I6" s="237"/>
+      <c r="B6" s="239"/>
+      <c r="C6" s="239"/>
+      <c r="D6" s="239"/>
+      <c r="E6" s="239"/>
+      <c r="F6" s="239"/>
+      <c r="G6" s="239"/>
+      <c r="H6" s="239"/>
+      <c r="I6" s="239"/>
       <c r="J6" s="123"/>
       <c r="L6" s="125"/>
       <c r="M6" s="125"/>
@@ -83989,17 +83969,17 @@
       </c>
     </row>
     <row r="12" spans="1:14" s="126" customFormat="1" ht="15" customHeight="1">
-      <c r="A12" s="237" t="s">
+      <c r="A12" s="239" t="s">
         <v>516</v>
       </c>
-      <c r="B12" s="237"/>
-      <c r="C12" s="237"/>
-      <c r="D12" s="237"/>
-      <c r="E12" s="237"/>
-      <c r="F12" s="237"/>
-      <c r="G12" s="237"/>
-      <c r="H12" s="237"/>
-      <c r="I12" s="237"/>
+      <c r="B12" s="239"/>
+      <c r="C12" s="239"/>
+      <c r="D12" s="239"/>
+      <c r="E12" s="239"/>
+      <c r="F12" s="239"/>
+      <c r="G12" s="239"/>
+      <c r="H12" s="239"/>
+      <c r="I12" s="239"/>
       <c r="J12" s="123"/>
       <c r="L12" s="125"/>
       <c r="M12" s="125"/>
@@ -84214,17 +84194,17 @@
       </c>
     </row>
     <row r="17" spans="1:14" s="126" customFormat="1" ht="15" customHeight="1">
-      <c r="A17" s="238" t="s">
+      <c r="A17" s="240" t="s">
         <v>530</v>
       </c>
-      <c r="B17" s="238"/>
-      <c r="C17" s="238"/>
-      <c r="D17" s="238"/>
-      <c r="E17" s="238"/>
-      <c r="F17" s="238"/>
-      <c r="G17" s="238"/>
-      <c r="H17" s="238"/>
-      <c r="I17" s="238"/>
+      <c r="B17" s="240"/>
+      <c r="C17" s="240"/>
+      <c r="D17" s="240"/>
+      <c r="E17" s="240"/>
+      <c r="F17" s="240"/>
+      <c r="G17" s="240"/>
+      <c r="H17" s="240"/>
+      <c r="I17" s="240"/>
       <c r="J17" s="123"/>
       <c r="K17" s="124"/>
       <c r="L17" s="125"/>

</xml_diff>